<commit_message>
extração das fontes por subsistema (na classe Subsistemas()) agregação das rotinas de impressao no main
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -3,10 +3,11 @@
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:workbookPr codeName="ThisWorkbook"/>
   <s:bookViews>
-    <s:workbookView activeTab="0"/>
+    <s:workbookView activeTab="1"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="Tabela1" sheetId="1" r:id="rId1"/>
+    <s:sheet name="pag2" sheetId="2" r:id="rId2"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -670,7 +671,7 @@
   </sheetPr>
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1256,41 +1257,117 @@
       <c r="Q14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="R14" t="s"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="n"/>
-      <c r="D15" s="1" t="n"/>
-      <c r="E15" s="1" t="n"/>
-      <c r="F15" s="1" t="n"/>
-      <c r="G15" s="1" t="n"/>
-      <c r="I15" s="1" t="n"/>
-      <c r="J15" s="1" t="n"/>
-      <c r="K15" s="1" t="n"/>
-      <c r="L15" s="1" t="n"/>
-      <c r="M15" s="1" t="n"/>
-      <c r="N15" s="1" t="n"/>
-      <c r="O15" s="1" t="n"/>
-      <c r="Q15" s="1" t="n"/>
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="B16" s="1" t="n"/>
-      <c r="C16" s="1" t="n"/>
-      <c r="D16" s="1" t="n"/>
-      <c r="E16" s="1" t="n"/>
-      <c r="F16" s="1" t="n"/>
-      <c r="G16" s="1" t="n"/>
-      <c r="I16" s="1" t="n"/>
-      <c r="J16" s="1" t="n"/>
-      <c r="K16" s="1" t="n"/>
-      <c r="L16" s="1" t="n"/>
-      <c r="M16" s="1" t="n"/>
-      <c r="N16" s="1" t="n"/>
-      <c r="O16" s="1" t="n"/>
-      <c r="Q16" s="1" t="n"/>
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P16" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="n"/>
@@ -1307,70 +1384,221 @@
       <c r="Q17" s="1" t="n"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="n"/>
-      <c r="D18" s="1" t="n"/>
-      <c r="E18" s="1" t="n"/>
-      <c r="F18" s="1" t="n"/>
-      <c r="G18" s="1" t="n"/>
-      <c r="I18" s="1" t="n"/>
-      <c r="J18" s="1" t="n"/>
-      <c r="K18" s="1" t="n"/>
-      <c r="L18" s="1" t="n"/>
-      <c r="M18" s="1" t="n"/>
-      <c r="N18" s="1" t="n"/>
-      <c r="O18" s="1" t="n"/>
-      <c r="Q18" s="1" t="n"/>
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P18" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="n"/>
-      <c r="D19" s="1" t="n"/>
-      <c r="E19" s="1" t="n"/>
-      <c r="F19" s="1" t="n"/>
-      <c r="G19" s="1" t="n"/>
-      <c r="I19" s="1" t="n"/>
-      <c r="J19" s="1" t="n"/>
-      <c r="K19" s="1" t="n"/>
-      <c r="L19" s="1" t="n"/>
-      <c r="M19" s="1" t="n"/>
-      <c r="N19" s="1" t="n"/>
-      <c r="O19" s="1" t="n"/>
-      <c r="Q19" s="1" t="n"/>
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P19" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="n"/>
-      <c r="D20" s="1" t="n"/>
-      <c r="E20" s="1" t="n"/>
-      <c r="F20" s="1" t="n"/>
-      <c r="G20" s="1" t="n"/>
-      <c r="I20" s="1" t="n"/>
-      <c r="J20" s="1" t="n"/>
-      <c r="K20" s="1" t="n"/>
-      <c r="L20" s="1" t="n"/>
-      <c r="M20" s="1" t="n"/>
-      <c r="N20" s="1" t="n"/>
-      <c r="O20" s="1" t="n"/>
-      <c r="Q20" s="1" t="n"/>
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P20" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="n"/>
-      <c r="D21" s="1" t="n"/>
-      <c r="E21" s="1" t="n"/>
-      <c r="F21" s="1" t="n"/>
-      <c r="G21" s="1" t="n"/>
-      <c r="I21" s="1" t="n"/>
-      <c r="J21" s="1" t="n"/>
-      <c r="K21" s="1" t="n"/>
-      <c r="L21" s="1" t="n"/>
-      <c r="M21" s="1" t="n"/>
-      <c r="N21" s="1" t="n"/>
-      <c r="O21" s="1" t="n"/>
-      <c r="Q21" s="1" t="n"/>
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P21" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="22" spans="1:18">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
       <c r="B22" s="1" t="n"/>
       <c r="C22" s="1" t="n"/>
       <c r="D22" s="1" t="n"/>
@@ -1387,68 +1615,217 @@
       <c r="Q22" s="1" t="n"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="B23" s="1" t="n"/>
-      <c r="C23" s="1" t="n"/>
-      <c r="D23" s="1" t="n"/>
-      <c r="E23" s="1" t="n"/>
-      <c r="F23" s="1" t="n"/>
-      <c r="G23" s="1" t="n"/>
-      <c r="I23" s="1" t="n"/>
-      <c r="J23" s="1" t="n"/>
-      <c r="K23" s="1" t="n"/>
-      <c r="L23" s="1" t="n"/>
-      <c r="M23" s="1" t="n"/>
-      <c r="N23" s="1" t="n"/>
-      <c r="O23" s="1" t="n"/>
-      <c r="Q23" s="1" t="n"/>
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P23" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="B24" s="1" t="n"/>
-      <c r="C24" s="1" t="n"/>
-      <c r="D24" s="1" t="n"/>
-      <c r="E24" s="1" t="n"/>
-      <c r="F24" s="1" t="n"/>
-      <c r="G24" s="1" t="n"/>
-      <c r="I24" s="1" t="n"/>
-      <c r="J24" s="1" t="n"/>
-      <c r="K24" s="1" t="n"/>
-      <c r="L24" s="1" t="n"/>
-      <c r="M24" s="1" t="n"/>
-      <c r="N24" s="1" t="n"/>
-      <c r="O24" s="1" t="n"/>
-      <c r="Q24" s="1" t="n"/>
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P24" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
-      <c r="D25" s="1" t="n"/>
-      <c r="E25" s="1" t="n"/>
-      <c r="F25" s="1" t="n"/>
-      <c r="G25" s="1" t="n"/>
-      <c r="I25" s="1" t="n"/>
-      <c r="J25" s="1" t="n"/>
-      <c r="K25" s="1" t="n"/>
-      <c r="L25" s="1" t="n"/>
-      <c r="M25" s="1" t="n"/>
-      <c r="N25" s="1" t="n"/>
-      <c r="O25" s="1" t="n"/>
-      <c r="Q25" s="1" t="n"/>
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P25" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n"/>
-      <c r="D26" s="1" t="n"/>
-      <c r="E26" s="1" t="n"/>
-      <c r="F26" s="1" t="n"/>
-      <c r="G26" s="1" t="n"/>
-      <c r="I26" s="1" t="n"/>
-      <c r="J26" s="1" t="n"/>
-      <c r="K26" s="1" t="n"/>
-      <c r="L26" s="1" t="n"/>
-      <c r="M26" s="1" t="n"/>
-      <c r="N26" s="1" t="n"/>
-      <c r="O26" s="1" t="n"/>
-      <c r="Q26" s="1" t="n"/>
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P26" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R26" t="s"/>
     </row>
     <row r="27" spans="1:18">
       <c r="B27" s="1" t="n"/>
@@ -1603,4 +1980,22 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="4294967293" orientation="portrait" paperSize="9" verticalDpi="4294967293"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mapeando os dados do sudeste (balanço detalhado)
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>Programado</t>
   </si>
@@ -204,6 +204,30 @@
   </si>
   <si>
     <t>62.823</t>
+  </si>
+  <si>
+    <t>Sudeste</t>
+  </si>
+  <si>
+    <t>Sul</t>
+  </si>
+  <si>
+    <t>Nordeste</t>
+  </si>
+  <si>
+    <t>Norte</t>
+  </si>
+  <si>
+    <t>Ghidro</t>
+  </si>
+  <si>
+    <t>Gtermo</t>
+  </si>
+  <si>
+    <t>Geólica</t>
+  </si>
+  <si>
+    <t>Gsolar</t>
   </si>
 </sst>
 </file>
@@ -248,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -338,11 +362,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="3" xfId="0"/>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -369,6 +430,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -669,10 +745,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1825,57 +1901,170 @@
       <c r="Q26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R26" t="s"/>
     </row>
     <row r="27" spans="1:18">
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="1" t="n"/>
-      <c r="D27" s="1" t="n"/>
-      <c r="E27" s="1" t="n"/>
-      <c r="F27" s="1" t="n"/>
-      <c r="G27" s="1" t="n"/>
-      <c r="I27" s="1" t="n"/>
-      <c r="J27" s="1" t="n"/>
-      <c r="K27" s="1" t="n"/>
-      <c r="L27" s="1" t="n"/>
-      <c r="M27" s="1" t="n"/>
-      <c r="N27" s="1" t="n"/>
-      <c r="O27" s="1" t="n"/>
-      <c r="Q27" s="1" t="n"/>
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P27" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" spans="1:18">
-      <c r="B28" s="1" t="n"/>
-      <c r="C28" s="1" t="n"/>
-      <c r="D28" s="1" t="n"/>
-      <c r="E28" s="1" t="n"/>
-      <c r="F28" s="1" t="n"/>
-      <c r="G28" s="1" t="n"/>
-      <c r="I28" s="1" t="n"/>
-      <c r="J28" s="1" t="n"/>
-      <c r="K28" s="1" t="n"/>
-      <c r="L28" s="1" t="n"/>
-      <c r="M28" s="1" t="n"/>
-      <c r="N28" s="1" t="n"/>
-      <c r="O28" s="1" t="n"/>
-      <c r="Q28" s="1" t="n"/>
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P28" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="B29" s="1" t="n"/>
-      <c r="C29" s="1" t="n"/>
-      <c r="D29" s="1" t="n"/>
-      <c r="E29" s="1" t="n"/>
-      <c r="F29" s="1" t="n"/>
-      <c r="G29" s="1" t="n"/>
-      <c r="I29" s="1" t="n"/>
-      <c r="J29" s="1" t="n"/>
-      <c r="K29" s="1" t="n"/>
-      <c r="L29" s="1" t="n"/>
-      <c r="M29" s="1" t="n"/>
-      <c r="N29" s="1" t="n"/>
-      <c r="O29" s="1" t="n"/>
-      <c r="Q29" s="1" t="n"/>
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P29" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="30" spans="1:18">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
       <c r="B30" s="1" t="n"/>
       <c r="C30" s="1" t="n"/>
       <c r="D30" s="1" t="n"/>
@@ -1892,85 +2081,641 @@
       <c r="Q30" s="1" t="n"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="B31" s="1" t="n"/>
-      <c r="C31" s="1" t="n"/>
-      <c r="D31" s="1" t="n"/>
-      <c r="E31" s="1" t="n"/>
-      <c r="F31" s="1" t="n"/>
-      <c r="G31" s="1" t="n"/>
-      <c r="I31" s="1" t="n"/>
-      <c r="J31" s="1" t="n"/>
-      <c r="K31" s="1" t="n"/>
-      <c r="L31" s="1" t="n"/>
-      <c r="M31" s="1" t="n"/>
-      <c r="N31" s="1" t="n"/>
-      <c r="O31" s="1" t="n"/>
-      <c r="Q31" s="1" t="n"/>
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P31" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="B32" s="1" t="n"/>
-      <c r="C32" s="1" t="n"/>
-      <c r="D32" s="1" t="n"/>
-      <c r="E32" s="1" t="n"/>
-      <c r="F32" s="1" t="n"/>
-      <c r="G32" s="1" t="n"/>
-      <c r="I32" s="1" t="n"/>
-      <c r="J32" s="1" t="n"/>
-      <c r="K32" s="1" t="n"/>
-      <c r="L32" s="1" t="n"/>
-      <c r="M32" s="1" t="n"/>
-      <c r="N32" s="1" t="n"/>
-      <c r="O32" s="1" t="n"/>
-      <c r="Q32" s="1" t="n"/>
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P32" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="B33" s="1" t="n"/>
-      <c r="C33" s="1" t="n"/>
-      <c r="D33" s="1" t="n"/>
-      <c r="E33" s="1" t="n"/>
-      <c r="F33" s="1" t="n"/>
-      <c r="G33" s="1" t="n"/>
-      <c r="I33" s="1" t="n"/>
-      <c r="J33" s="1" t="n"/>
-      <c r="K33" s="1" t="n"/>
-      <c r="L33" s="1" t="n"/>
-      <c r="M33" s="1" t="n"/>
-      <c r="N33" s="1" t="n"/>
-      <c r="O33" s="1" t="n"/>
-      <c r="Q33" s="1" t="n"/>
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P33" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="34" spans="1:18">
-      <c r="B34" s="1" t="n"/>
-      <c r="C34" s="1" t="n"/>
-      <c r="D34" s="1" t="n"/>
-      <c r="E34" s="1" t="n"/>
-      <c r="F34" s="1" t="n"/>
-      <c r="G34" s="1" t="n"/>
-      <c r="I34" s="1" t="n"/>
-      <c r="J34" s="1" t="n"/>
-      <c r="K34" s="1" t="n"/>
-      <c r="L34" s="1" t="n"/>
-      <c r="M34" s="1" t="n"/>
-      <c r="N34" s="1" t="n"/>
-      <c r="O34" s="1" t="n"/>
-      <c r="Q34" s="1" t="n"/>
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P34" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="35" spans="1:18">
-      <c r="B35" s="1" t="n"/>
-      <c r="C35" s="1" t="n"/>
-      <c r="D35" s="1" t="n"/>
-      <c r="E35" s="1" t="n"/>
-      <c r="F35" s="1" t="n"/>
-      <c r="G35" s="1" t="n"/>
-      <c r="H35" s="1" t="n"/>
-      <c r="I35" s="1" t="n"/>
-      <c r="J35" s="1" t="n"/>
-      <c r="K35" s="1" t="n"/>
-      <c r="L35" s="1" t="n"/>
-      <c r="M35" s="1" t="n"/>
-      <c r="N35" s="1" t="n"/>
-      <c r="O35" s="1" t="n"/>
-      <c r="Q35" s="1" t="n"/>
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P35" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" t="s">
+        <v>23</v>
+      </c>
+      <c r="O36" t="s">
+        <v>24</v>
+      </c>
+      <c r="P36" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37" t="s">
+        <v>23</v>
+      </c>
+      <c r="O37" t="s">
+        <v>24</v>
+      </c>
+      <c r="P37" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" t="s">
+        <v>21</v>
+      </c>
+      <c r="M38" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38" t="s">
+        <v>23</v>
+      </c>
+      <c r="O38" t="s">
+        <v>24</v>
+      </c>
+      <c r="P38" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" t="s">
+        <v>22</v>
+      </c>
+      <c r="N39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O39" t="s">
+        <v>24</v>
+      </c>
+      <c r="P39" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" t="s">
+        <v>22</v>
+      </c>
+      <c r="N40" t="s">
+        <v>23</v>
+      </c>
+      <c r="O40" t="s">
+        <v>24</v>
+      </c>
+      <c r="P40" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" t="s">
+        <v>20</v>
+      </c>
+      <c r="L41" t="s">
+        <v>21</v>
+      </c>
+      <c r="M41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N41" t="s">
+        <v>23</v>
+      </c>
+      <c r="O41" t="s">
+        <v>24</v>
+      </c>
+      <c r="P41" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" t="s">
+        <v>21</v>
+      </c>
+      <c r="M42" t="s">
+        <v>22</v>
+      </c>
+      <c r="N42" t="s">
+        <v>23</v>
+      </c>
+      <c r="O42" t="s">
+        <v>24</v>
+      </c>
+      <c r="P42" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>24</v>
+      </c>
+      <c r="R42" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1988,14 +2733,119 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A3:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="7" width="16.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:21">
+      <c r="B3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="15" t="n"/>
+      <c r="D3" s="15" t="n"/>
+      <c r="E3" s="15" t="n"/>
+      <c r="F3" s="16" t="n"/>
+      <c r="G3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="15" t="n"/>
+      <c r="I3" s="15" t="n"/>
+      <c r="J3" s="15" t="n"/>
+      <c r="K3" s="16" t="n"/>
+      <c r="L3" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="15" t="n"/>
+      <c r="N3" s="15" t="n"/>
+      <c r="O3" s="15" t="n"/>
+      <c r="P3" s="16" t="n"/>
+      <c r="Q3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="13" t="n"/>
+      <c r="S3" s="13" t="n"/>
+      <c r="T3" s="13" t="n"/>
+      <c r="U3" s="13" t="n"/>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+  </mergeCells>
   <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mapeamento do balanço energético detalhado
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -745,7 +745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -2715,7 +2715,325 @@
       <c r="Q42" t="s">
         <v>24</v>
       </c>
-      <c r="R42" t="s"/>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" t="s">
+        <v>21</v>
+      </c>
+      <c r="M43" t="s">
+        <v>22</v>
+      </c>
+      <c r="N43" t="s">
+        <v>23</v>
+      </c>
+      <c r="O43" t="s">
+        <v>24</v>
+      </c>
+      <c r="P43" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L44" t="s">
+        <v>21</v>
+      </c>
+      <c r="M44" t="s">
+        <v>22</v>
+      </c>
+      <c r="N44" t="s">
+        <v>23</v>
+      </c>
+      <c r="O44" t="s">
+        <v>24</v>
+      </c>
+      <c r="P44" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" t="s">
+        <v>21</v>
+      </c>
+      <c r="M45" t="s">
+        <v>22</v>
+      </c>
+      <c r="N45" t="s">
+        <v>23</v>
+      </c>
+      <c r="O45" t="s">
+        <v>24</v>
+      </c>
+      <c r="P45" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" t="s">
+        <v>19</v>
+      </c>
+      <c r="K46" t="s">
+        <v>20</v>
+      </c>
+      <c r="L46" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46" t="s">
+        <v>22</v>
+      </c>
+      <c r="N46" t="s">
+        <v>23</v>
+      </c>
+      <c r="O46" t="s">
+        <v>24</v>
+      </c>
+      <c r="P46" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K47" t="s">
+        <v>20</v>
+      </c>
+      <c r="L47" t="s">
+        <v>21</v>
+      </c>
+      <c r="M47" t="s">
+        <v>22</v>
+      </c>
+      <c r="N47" t="s">
+        <v>23</v>
+      </c>
+      <c r="O47" t="s">
+        <v>24</v>
+      </c>
+      <c r="P47" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" t="s">
+        <v>19</v>
+      </c>
+      <c r="K48" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" t="s">
+        <v>21</v>
+      </c>
+      <c r="M48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N48" t="s">
+        <v>23</v>
+      </c>
+      <c r="O48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P48" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>24</v>
+      </c>
+      <c r="R48" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Revisando as expressões regulares da classe Mapeamento(antigo DicionarioTexto)
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -3,7 +3,7 @@
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:workbookPr codeName="ThisWorkbook"/>
   <s:bookViews>
-    <s:workbookView activeTab="1"/>
+    <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="Tabela1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>Programado</t>
   </si>
@@ -204,6 +204,75 @@
   </si>
   <si>
     <t>62.823</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 Maio de 2016</t>
+  </si>
+  <si>
+    <t>36.999</t>
+  </si>
+  <si>
+    <t>11.816</t>
+  </si>
+  <si>
+    <t>8.070</t>
+  </si>
+  <si>
+    <t>3.730</t>
+  </si>
+  <si>
+    <t>62.605</t>
+  </si>
+  <si>
+    <t>37.552</t>
+  </si>
+  <si>
+    <t>11.869</t>
+  </si>
+  <si>
+    <t>2.013</t>
+  </si>
+  <si>
+    <t>7.552</t>
+  </si>
+  <si>
+    <t>3.946</t>
+  </si>
+  <si>
+    <t>62.932</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 Maio de 2016</t>
+  </si>
+  <si>
+    <t>32.860</t>
+  </si>
+  <si>
+    <t>10.265</t>
+  </si>
+  <si>
+    <t>8.943</t>
+  </si>
+  <si>
+    <t>3.546</t>
+  </si>
+  <si>
+    <t>57.604</t>
+  </si>
+  <si>
+    <t>33.585</t>
+  </si>
+  <si>
+    <t>10.612</t>
+  </si>
+  <si>
+    <t>8.445</t>
+  </si>
+  <si>
+    <t>3.243</t>
+  </si>
+  <si>
+    <t>57.898</t>
   </si>
   <si>
     <t>Sudeste</t>
@@ -420,6 +489,9 @@
     </xf>
     <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -430,9 +502,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -745,10 +814,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -764,26 +833,26 @@
     <row r="1" spans="1:18"/>
     <row r="2" spans="1:18"/>
     <row customHeight="1" ht="16.5" r="3" s="7" spans="1:18">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="n"/>
-      <c r="D3" s="9" t="n"/>
-      <c r="E3" s="9" t="n"/>
-      <c r="F3" s="9" t="n"/>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="9" t="n"/>
-      <c r="I3" s="9" t="n"/>
-      <c r="J3" s="10" t="s">
+      <c r="C3" s="10" t="n"/>
+      <c r="D3" s="10" t="n"/>
+      <c r="E3" s="10" t="n"/>
+      <c r="F3" s="10" t="n"/>
+      <c r="G3" s="10" t="n"/>
+      <c r="H3" s="10" t="n"/>
+      <c r="I3" s="10" t="n"/>
+      <c r="J3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="11" t="n"/>
-      <c r="L3" s="11" t="n"/>
-      <c r="M3" s="11" t="n"/>
-      <c r="N3" s="11" t="n"/>
-      <c r="O3" s="11" t="n"/>
-      <c r="P3" s="11" t="n"/>
-      <c r="Q3" s="11" t="n"/>
+      <c r="K3" s="12" t="n"/>
+      <c r="L3" s="12" t="n"/>
+      <c r="M3" s="12" t="n"/>
+      <c r="N3" s="12" t="n"/>
+      <c r="O3" s="12" t="n"/>
+      <c r="P3" s="12" t="n"/>
+      <c r="Q3" s="12" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="4" s="7" spans="1:18">
       <c r="A4" s="6" t="s">
@@ -3033,7 +3102,653 @@
       <c r="Q48" t="s">
         <v>24</v>
       </c>
-      <c r="R48" t="s"/>
+    </row>
+    <row r="49" spans="1:18">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" t="s">
+        <v>19</v>
+      </c>
+      <c r="K49" t="s">
+        <v>20</v>
+      </c>
+      <c r="L49" t="s">
+        <v>21</v>
+      </c>
+      <c r="M49" t="s">
+        <v>22</v>
+      </c>
+      <c r="N49" t="s">
+        <v>23</v>
+      </c>
+      <c r="O49" t="s">
+        <v>24</v>
+      </c>
+      <c r="P49" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51" t="s">
+        <v>21</v>
+      </c>
+      <c r="M51" t="s">
+        <v>22</v>
+      </c>
+      <c r="N51" t="s">
+        <v>23</v>
+      </c>
+      <c r="O51" t="s">
+        <v>24</v>
+      </c>
+      <c r="P51" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" t="s">
+        <v>20</v>
+      </c>
+      <c r="L52" t="s">
+        <v>21</v>
+      </c>
+      <c r="M52" t="s">
+        <v>22</v>
+      </c>
+      <c r="N52" t="s">
+        <v>23</v>
+      </c>
+      <c r="O52" t="s">
+        <v>24</v>
+      </c>
+      <c r="P52" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" t="s">
+        <v>20</v>
+      </c>
+      <c r="L54" t="s">
+        <v>21</v>
+      </c>
+      <c r="M54" t="s">
+        <v>22</v>
+      </c>
+      <c r="N54" t="s">
+        <v>23</v>
+      </c>
+      <c r="O54" t="s">
+        <v>24</v>
+      </c>
+      <c r="P54" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" t="s">
+        <v>19</v>
+      </c>
+      <c r="K55" t="s">
+        <v>20</v>
+      </c>
+      <c r="L55" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55" t="s">
+        <v>22</v>
+      </c>
+      <c r="N55" t="s">
+        <v>23</v>
+      </c>
+      <c r="O55" t="s">
+        <v>24</v>
+      </c>
+      <c r="P55" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" t="s">
+        <v>30</v>
+      </c>
+      <c r="H56" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" t="s">
+        <v>30</v>
+      </c>
+      <c r="J56" t="s">
+        <v>31</v>
+      </c>
+      <c r="K56" t="s">
+        <v>32</v>
+      </c>
+      <c r="L56" t="s">
+        <v>21</v>
+      </c>
+      <c r="M56" t="s">
+        <v>33</v>
+      </c>
+      <c r="N56" t="s">
+        <v>34</v>
+      </c>
+      <c r="O56" t="s">
+        <v>35</v>
+      </c>
+      <c r="P56" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>66</v>
+      </c>
+      <c r="F57" t="s">
+        <v>67</v>
+      </c>
+      <c r="G57" t="s">
+        <v>68</v>
+      </c>
+      <c r="H57" t="s">
+        <v>18</v>
+      </c>
+      <c r="I57" t="s">
+        <v>68</v>
+      </c>
+      <c r="J57" t="s">
+        <v>69</v>
+      </c>
+      <c r="K57" t="s">
+        <v>70</v>
+      </c>
+      <c r="L57" t="s">
+        <v>71</v>
+      </c>
+      <c r="M57" t="s">
+        <v>72</v>
+      </c>
+      <c r="N57" t="s">
+        <v>73</v>
+      </c>
+      <c r="O57" t="s">
+        <v>74</v>
+      </c>
+      <c r="P57" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s">
+        <v>78</v>
+      </c>
+      <c r="F58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" t="s">
+        <v>80</v>
+      </c>
+      <c r="H58" t="s">
+        <v>18</v>
+      </c>
+      <c r="I58" t="s">
+        <v>80</v>
+      </c>
+      <c r="J58" t="s">
+        <v>81</v>
+      </c>
+      <c r="K58" t="s">
+        <v>82</v>
+      </c>
+      <c r="L58" t="s">
+        <v>71</v>
+      </c>
+      <c r="M58" t="s">
+        <v>83</v>
+      </c>
+      <c r="N58" t="s">
+        <v>84</v>
+      </c>
+      <c r="O58" t="s">
+        <v>85</v>
+      </c>
+      <c r="P58" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" t="s">
+        <v>66</v>
+      </c>
+      <c r="F59" t="s">
+        <v>67</v>
+      </c>
+      <c r="G59" t="s">
+        <v>68</v>
+      </c>
+      <c r="H59" t="s">
+        <v>18</v>
+      </c>
+      <c r="I59" t="s">
+        <v>68</v>
+      </c>
+      <c r="J59" t="s">
+        <v>69</v>
+      </c>
+      <c r="K59" t="s">
+        <v>70</v>
+      </c>
+      <c r="L59" t="s">
+        <v>71</v>
+      </c>
+      <c r="M59" t="s">
+        <v>72</v>
+      </c>
+      <c r="N59" t="s">
+        <v>73</v>
+      </c>
+      <c r="O59" t="s">
+        <v>74</v>
+      </c>
+      <c r="P59" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="A60" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" t="s">
+        <v>78</v>
+      </c>
+      <c r="F60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G60" t="s">
+        <v>80</v>
+      </c>
+      <c r="H60" t="s">
+        <v>18</v>
+      </c>
+      <c r="I60" t="s">
+        <v>80</v>
+      </c>
+      <c r="J60" t="s">
+        <v>81</v>
+      </c>
+      <c r="K60" t="s">
+        <v>82</v>
+      </c>
+      <c r="L60" t="s">
+        <v>71</v>
+      </c>
+      <c r="M60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N60" t="s">
+        <v>84</v>
+      </c>
+      <c r="O60" t="s">
+        <v>85</v>
+      </c>
+      <c r="P60" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" t="s">
+        <v>66</v>
+      </c>
+      <c r="F61" t="s">
+        <v>67</v>
+      </c>
+      <c r="G61" t="s">
+        <v>68</v>
+      </c>
+      <c r="H61" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" t="s">
+        <v>68</v>
+      </c>
+      <c r="J61" t="s">
+        <v>69</v>
+      </c>
+      <c r="K61" t="s">
+        <v>70</v>
+      </c>
+      <c r="L61" t="s">
+        <v>71</v>
+      </c>
+      <c r="M61" t="s">
+        <v>72</v>
+      </c>
+      <c r="N61" t="s">
+        <v>73</v>
+      </c>
+      <c r="O61" t="s">
+        <v>74</v>
+      </c>
+      <c r="P61" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="A62" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" t="s">
+        <v>78</v>
+      </c>
+      <c r="F62" t="s">
+        <v>79</v>
+      </c>
+      <c r="G62" t="s">
+        <v>80</v>
+      </c>
+      <c r="H62" t="s">
+        <v>18</v>
+      </c>
+      <c r="I62" t="s">
+        <v>80</v>
+      </c>
+      <c r="J62" t="s">
+        <v>81</v>
+      </c>
+      <c r="K62" t="s">
+        <v>82</v>
+      </c>
+      <c r="L62" t="s">
+        <v>71</v>
+      </c>
+      <c r="M62" t="s">
+        <v>83</v>
+      </c>
+      <c r="N62" t="s">
+        <v>84</v>
+      </c>
+      <c r="O62" t="s">
+        <v>85</v>
+      </c>
+      <c r="P62" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>85</v>
+      </c>
+      <c r="R62" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3053,7 +3768,7 @@
   </sheetPr>
   <dimension ref="A3:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3:U3"/>
     </sheetView>
   </sheetViews>
@@ -3064,28 +3779,28 @@
   <sheetData>
     <row r="3" spans="1:21">
       <c r="B3" s="14" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C3" s="15" t="n"/>
       <c r="D3" s="15" t="n"/>
       <c r="E3" s="15" t="n"/>
       <c r="F3" s="16" t="n"/>
       <c r="G3" s="14" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="H3" s="15" t="n"/>
       <c r="I3" s="15" t="n"/>
       <c r="J3" s="15" t="n"/>
       <c r="K3" s="16" t="n"/>
       <c r="L3" s="14" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="M3" s="15" t="n"/>
       <c r="N3" s="15" t="n"/>
       <c r="O3" s="15" t="n"/>
       <c r="P3" s="16" t="n"/>
       <c r="Q3" s="13" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="R3" s="13" t="n"/>
       <c r="S3" s="13" t="n"/>
@@ -3097,61 +3812,61 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="P4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="U4" s="13" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
RegEx revisadas refactory em balanco_por_subsistema algumas modificações em balanco_energetico_detalhado
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
   <si>
     <t>Programado</t>
   </si>
@@ -273,6 +273,39 @@
   </si>
   <si>
     <t>57.898</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22 Maio de 2016</t>
+  </si>
+  <si>
+    <t>29.037</t>
+  </si>
+  <si>
+    <t>9.653</t>
+  </si>
+  <si>
+    <t>8.234</t>
+  </si>
+  <si>
+    <t>3.556</t>
+  </si>
+  <si>
+    <t>52.470</t>
+  </si>
+  <si>
+    <t>29.472</t>
+  </si>
+  <si>
+    <t>9.636</t>
+  </si>
+  <si>
+    <t>7.888</t>
+  </si>
+  <si>
+    <t>3.313</t>
+  </si>
+  <si>
+    <t>52.324</t>
   </si>
   <si>
     <t>Sudeste</t>
@@ -814,7 +847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R62"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A54" sqref="A54:XFD54"/>
@@ -3748,7 +3781,60 @@
       <c r="Q62" t="s">
         <v>85</v>
       </c>
-      <c r="R62" t="s"/>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="A63" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" t="s">
+        <v>90</v>
+      </c>
+      <c r="G63" t="s">
+        <v>91</v>
+      </c>
+      <c r="H63" t="s">
+        <v>18</v>
+      </c>
+      <c r="I63" t="s">
+        <v>91</v>
+      </c>
+      <c r="J63" t="s">
+        <v>92</v>
+      </c>
+      <c r="K63" t="s">
+        <v>93</v>
+      </c>
+      <c r="L63" t="s">
+        <v>21</v>
+      </c>
+      <c r="M63" t="s">
+        <v>94</v>
+      </c>
+      <c r="N63" t="s">
+        <v>95</v>
+      </c>
+      <c r="O63" t="s">
+        <v>96</v>
+      </c>
+      <c r="P63" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>96</v>
+      </c>
+      <c r="R63" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3779,28 +3865,28 @@
   <sheetData>
     <row r="3" spans="1:21">
       <c r="B3" s="14" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C3" s="15" t="n"/>
       <c r="D3" s="15" t="n"/>
       <c r="E3" s="15" t="n"/>
       <c r="F3" s="16" t="n"/>
       <c r="G3" s="14" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="H3" s="15" t="n"/>
       <c r="I3" s="15" t="n"/>
       <c r="J3" s="15" t="n"/>
       <c r="K3" s="16" t="n"/>
       <c r="L3" s="14" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="M3" s="15" t="n"/>
       <c r="N3" s="15" t="n"/>
       <c r="O3" s="15" t="n"/>
       <c r="P3" s="16" t="n"/>
       <c r="Q3" s="13" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="R3" s="13" t="n"/>
       <c r="S3" s="13" t="n"/>
@@ -3812,61 +3898,61 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="P4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="U4" s="13" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
refactory em DadosBalancoEnergeticoDetalhado tirando os splits e inserindo um único split dados_objeto_bs
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudio\Documents\Python\ETL_PDF\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="11955" activeTab="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Tabela1" sheetId="1" r:id="rId1"/>
-    <sheet name="BalancoEnergeticoDetalhado" sheetId="2" r:id="rId2"/>
-  </sheets>
-  <calcPr calcId="0"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="1"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Tabela1" sheetId="1" r:id="rId1"/>
+    <s:sheet name="BalancoEnergeticoDetalhado" sheetId="2" r:id="rId2"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
   <si>
     <t>Programado</t>
   </si>
@@ -334,43 +329,82 @@
     <t>Gtermo</t>
   </si>
   <si>
+    <t>Gnuclear</t>
+  </si>
+  <si>
     <t>Geólica</t>
   </si>
   <si>
     <t>Gsolar</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>hoje</t>
+  </si>
+  <si>
+    <t>14.528</t>
+  </si>
+  <si>
+    <t>3.746</t>
+  </si>
+  <si>
+    <t>20.289</t>
+  </si>
+  <si>
+    <t>30.185</t>
+  </si>
+  <si>
+    <t>13.657</t>
+  </si>
+  <si>
+    <t>4.651</t>
+  </si>
+  <si>
+    <t>20.323</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,8 +414,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.3999755851924192"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -475,11 +521,24 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -487,89 +546,88 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="20">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="3" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="7" fillId="5" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="7" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -857,46 +915,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A3:Q79"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="7" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="12" width="16.42578125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="12" width="14.140625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="12" width="11.5703125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="12" width="16.5703125"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="12" width="14.140625"/>
+    <col customWidth="1" max="13" min="13" style="12" width="12.140625"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+    <row customHeight="1" ht="16.5" r="3" s="12" spans="1:17">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11" t="s">
+      <c r="C3" s="14" t="n"/>
+      <c r="D3" s="14" t="n"/>
+      <c r="E3" s="14" t="n"/>
+      <c r="F3" s="14" t="n"/>
+      <c r="G3" s="14" t="n"/>
+      <c r="H3" s="14" t="n"/>
+      <c r="I3" s="14" t="n"/>
+      <c r="J3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="16" t="n"/>
+      <c r="L3" s="16" t="n"/>
+      <c r="M3" s="16" t="n"/>
+      <c r="N3" s="16" t="n"/>
+      <c r="O3" s="16" t="n"/>
+      <c r="P3" s="16" t="n"/>
+      <c r="Q3" s="16" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="12" spans="1:17">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -949,7 +1011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1002,7 +1064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1055,7 +1117,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1108,7 +1170,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1161,7 +1223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1214,26 +1276,26 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="I10" s="1" t="n"/>
+      <c r="J10" s="1" t="n"/>
+      <c r="K10" s="1" t="n"/>
+      <c r="L10" s="1" t="n"/>
+      <c r="M10" s="1" t="n"/>
+      <c r="N10" s="1" t="n"/>
+      <c r="O10" s="1" t="n"/>
+      <c r="Q10" s="1" t="n"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1286,7 +1348,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1339,7 +1401,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1392,7 +1454,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1445,7 +1507,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1498,7 +1560,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1551,26 +1613,26 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="n"/>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
+      <c r="F17" s="1" t="n"/>
+      <c r="G17" s="1" t="n"/>
+      <c r="I17" s="1" t="n"/>
+      <c r="J17" s="1" t="n"/>
+      <c r="K17" s="1" t="n"/>
+      <c r="L17" s="1" t="n"/>
+      <c r="M17" s="1" t="n"/>
+      <c r="N17" s="1" t="n"/>
+      <c r="O17" s="1" t="n"/>
+      <c r="Q17" s="1" t="n"/>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1623,7 +1685,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1676,7 +1738,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1729,7 +1791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1782,26 +1844,26 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="n"/>
+      <c r="C22" s="1" t="n"/>
+      <c r="D22" s="1" t="n"/>
+      <c r="E22" s="1" t="n"/>
+      <c r="F22" s="1" t="n"/>
+      <c r="G22" s="1" t="n"/>
+      <c r="I22" s="1" t="n"/>
+      <c r="J22" s="1" t="n"/>
+      <c r="K22" s="1" t="n"/>
+      <c r="L22" s="1" t="n"/>
+      <c r="M22" s="1" t="n"/>
+      <c r="N22" s="1" t="n"/>
+      <c r="O22" s="1" t="n"/>
+      <c r="Q22" s="1" t="n"/>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1854,7 +1916,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1907,7 +1969,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1960,7 +2022,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -2013,7 +2075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2066,7 +2128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2119,7 +2181,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2172,26 +2234,26 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="Q30" s="1"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="1" t="n"/>
+      <c r="D30" s="1" t="n"/>
+      <c r="E30" s="1" t="n"/>
+      <c r="F30" s="1" t="n"/>
+      <c r="G30" s="1" t="n"/>
+      <c r="I30" s="1" t="n"/>
+      <c r="J30" s="1" t="n"/>
+      <c r="K30" s="1" t="n"/>
+      <c r="L30" s="1" t="n"/>
+      <c r="M30" s="1" t="n"/>
+      <c r="N30" s="1" t="n"/>
+      <c r="O30" s="1" t="n"/>
+      <c r="Q30" s="1" t="n"/>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2244,7 +2306,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2297,7 +2359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2350,7 +2412,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -2403,7 +2465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2456,7 +2518,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2509,7 +2571,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2562,7 +2624,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2615,7 +2677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2668,7 +2730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2721,7 +2783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2774,7 +2836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2827,7 +2889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2880,7 +2942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2933,7 +2995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2986,7 +3048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -3039,7 +3101,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -3092,7 +3154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -3145,7 +3207,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -3198,12 +3260,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -3256,7 +3318,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -3309,12 +3371,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -3367,7 +3429,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -3420,7 +3482,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -3473,7 +3535,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -3526,7 +3588,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>75</v>
       </c>
@@ -3579,7 +3641,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -3632,7 +3694,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -3685,7 +3747,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -3738,7 +3800,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -3791,7 +3853,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -3844,7 +3906,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -3897,7 +3959,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -3950,7 +4012,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -3979,12 +4041,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -4013,7 +4075,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -4042,7 +4104,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -4071,7 +4133,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -4124,12 +4186,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -4182,12 +4244,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -4240,7 +4302,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -4293,7 +4355,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -4346,7 +4408,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -4399,7 +4461,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -4457,126 +4519,362 @@
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="J3:Q3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" paperSize="9" verticalDpi="4294967293"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:U4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BE6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:U3"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="B5" xSplit="1" ySplit="4"/>
+      <selection activeCell="B1" pane="topRight" sqref="B1"/>
+      <selection activeCell="A5" pane="bottomLeft" sqref="A5"/>
+      <selection activeCell="A6" pane="bottomRight" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="12" width="16.42578125"/>
+    <col customWidth="1" max="4" min="4" style="12" width="11.42578125"/>
+    <col customWidth="1" max="14" min="7" style="12" width="11.42578125"/>
+    <col customWidth="1" max="18" min="18" style="12" width="11.42578125"/>
+    <col customWidth="1" max="21" min="21" style="12" width="11.42578125"/>
+    <col customWidth="1" max="27" min="27" style="12" width="11.42578125"/>
+    <col customWidth="1" max="33" min="33" style="12" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+    <row r="1" spans="1:57">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="2" s="12" spans="1:57">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="3" s="12" spans="1:57">
+      <c r="B3" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="14" t="s">
+      <c r="C3" s="18" t="n"/>
+      <c r="D3" s="18" t="n"/>
+      <c r="E3" s="18" t="n"/>
+      <c r="F3" s="18" t="n"/>
+      <c r="G3" s="18" t="n"/>
+      <c r="H3" s="18" t="n"/>
+      <c r="I3" s="18" t="n"/>
+      <c r="J3" s="18" t="n"/>
+      <c r="K3" s="18" t="n"/>
+      <c r="L3" s="18" t="n"/>
+      <c r="M3" s="18" t="n"/>
+      <c r="N3" s="18" t="n"/>
+      <c r="O3" s="19" t="n"/>
+      <c r="P3" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="14" t="s">
+      <c r="Q3" s="18" t="n"/>
+      <c r="R3" s="18" t="n"/>
+      <c r="S3" s="18" t="n"/>
+      <c r="T3" s="18" t="n"/>
+      <c r="U3" s="18" t="n"/>
+      <c r="V3" s="18" t="n"/>
+      <c r="W3" s="18" t="n"/>
+      <c r="X3" s="18" t="n"/>
+      <c r="Y3" s="18" t="n"/>
+      <c r="Z3" s="18" t="n"/>
+      <c r="AA3" s="18" t="n"/>
+      <c r="AB3" s="18" t="n"/>
+      <c r="AC3" s="19" t="n"/>
+      <c r="AD3" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="13" t="s">
+      <c r="AE3" s="18" t="n"/>
+      <c r="AF3" s="18" t="n"/>
+      <c r="AG3" s="18" t="n"/>
+      <c r="AH3" s="18" t="n"/>
+      <c r="AI3" s="18" t="n"/>
+      <c r="AJ3" s="18" t="n"/>
+      <c r="AK3" s="18" t="n"/>
+      <c r="AL3" s="18" t="n"/>
+      <c r="AM3" s="18" t="n"/>
+      <c r="AN3" s="18" t="n"/>
+      <c r="AO3" s="18" t="n"/>
+      <c r="AP3" s="18" t="n"/>
+      <c r="AQ3" s="19" t="n"/>
+      <c r="AR3" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="AS3" s="18" t="n"/>
+      <c r="AT3" s="18" t="n"/>
+      <c r="AU3" s="18" t="n"/>
+      <c r="AV3" s="18" t="n"/>
+      <c r="AW3" s="18" t="n"/>
+      <c r="AX3" s="18" t="n"/>
+      <c r="AY3" s="18" t="n"/>
+      <c r="AZ3" s="18" t="n"/>
+      <c r="BA3" s="18" t="n"/>
+      <c r="BB3" s="18" t="n"/>
+      <c r="BC3" s="18" t="n"/>
+      <c r="BD3" s="18" t="n"/>
+      <c r="BE3" s="19" t="n"/>
+    </row>
+    <row r="4" spans="1:57">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="I4" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="J4" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="K4" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="L4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="M4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="P4" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="Q4" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="R4" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="S4" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="T4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="V4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="W4" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="X4" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="Y4" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="Z4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="AA4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC4" s="10" t="s">
         <v>10</v>
+      </c>
+      <c r="AD4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL4" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AM4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="AN4" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AO4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AP4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AQ4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AT4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AY4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AZ4" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="BA4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="BB4" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="BD4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="BE4" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="N5" s="7" t="n"/>
+      <c r="O5" s="7" t="n"/>
+      <c r="P5" s="7" t="n"/>
+      <c r="Q5" s="7" t="n"/>
+      <c r="S5" s="7" t="n"/>
+      <c r="U5" s="7" t="n"/>
+      <c r="V5" s="7" t="n"/>
+      <c r="W5" s="7" t="n"/>
+      <c r="X5" s="7" t="n"/>
+      <c r="Z5" s="7" t="n"/>
+      <c r="AB5" s="7" t="n"/>
+      <c r="AC5" s="7" t="n"/>
+      <c r="AD5" s="7" t="n"/>
+      <c r="AE5" s="7" t="n"/>
+      <c r="AG5" s="7" t="n"/>
+      <c r="AK5" s="7" t="n"/>
+      <c r="AL5" s="7" t="n"/>
+      <c r="AN5" s="7" t="n"/>
+      <c r="AP5" s="7" t="n"/>
+      <c r="AQ5" s="7" t="n"/>
+      <c r="AR5" s="7" t="n"/>
+      <c r="AS5" s="7" t="n"/>
+      <c r="AW5" s="7" t="n"/>
+      <c r="AX5" s="7" t="n"/>
+      <c r="AY5" s="7" t="n"/>
+      <c r="AZ5" s="7" t="n"/>
+      <c r="BD5" s="7" t="n"/>
+      <c r="BE5" s="7" t="n"/>
+    </row>
+    <row r="6" spans="1:57">
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="AR3:BE3"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="P3:AC3"/>
+    <mergeCell ref="AD3:AQ3"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" paperSize="9" verticalDpi="4294967293"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactory imprimir_resultados unindo imprimir_data_arquivo com balanco_energia_resumido_em_xlsx
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -3,7 +3,7 @@
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:workbookPr codeName="ThisWorkbook"/>
   <s:bookViews>
-    <s:workbookView activeTab="1"/>
+    <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="Tabela1" sheetId="1" r:id="rId1"/>
@@ -920,10 +920,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:Q79"/>
+  <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -936,7 +936,9 @@
     <col customWidth="1" max="13" min="13" style="12" width="12.140625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="16.5" r="3" s="12" spans="1:17">
+    <row r="1" spans="1:18"/>
+    <row r="2" spans="1:18"/>
+    <row customHeight="1" ht="16.5" r="3" s="12" spans="1:18">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
@@ -958,7 +960,7 @@
       <c r="P3" s="16" t="n"/>
       <c r="Q3" s="16" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="4" s="12" spans="1:17">
+    <row customHeight="1" ht="15.75" r="4" s="12" spans="1:18">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1117,7 +1119,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1170,7 +1172,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1223,7 +1225,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1276,7 +1278,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1295,7 +1297,7 @@
       <c r="O10" s="1" t="n"/>
       <c r="Q10" s="1" t="n"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1348,7 +1350,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1401,7 +1403,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1454,7 +1456,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1507,7 +1509,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1560,7 +1562,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1613,7 +1615,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1632,7 +1634,7 @@
       <c r="O17" s="1" t="n"/>
       <c r="Q17" s="1" t="n"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1685,7 +1687,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1738,7 +1740,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1791,7 +1793,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1863,7 +1865,7 @@
       <c r="O22" s="1" t="n"/>
       <c r="Q22" s="1" t="n"/>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1916,7 +1918,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1969,7 +1971,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2022,7 +2024,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -2075,7 +2077,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2128,7 +2130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2234,7 +2236,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:18">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2253,7 +2255,7 @@
       <c r="O30" s="1" t="n"/>
       <c r="Q30" s="1" t="n"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:18">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2306,7 +2308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:18">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2359,7 +2361,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:18">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2412,7 +2414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:18">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -2465,7 +2467,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:18">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2518,7 +2520,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:18">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2571,7 +2573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:18">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2624,7 +2626,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:18">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2677,7 +2679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:18">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2730,7 +2732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:18">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2783,7 +2785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:18">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2836,7 +2838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:18">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2889,7 +2891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:18">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2942,7 +2944,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:18">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2995,7 +2997,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:18">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -3048,7 +3050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:18">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -3101,7 +3103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:18">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -3154,7 +3156,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:18">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -3207,7 +3209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:18">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -3260,12 +3262,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:18">
       <c r="A50" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:18">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -3318,7 +3320,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:18">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -3371,12 +3373,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:18">
       <c r="A53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:18">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -3429,7 +3431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:18">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -3482,7 +3484,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:18">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -3535,7 +3537,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:18">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -3588,7 +3590,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:18">
       <c r="A58" t="s">
         <v>75</v>
       </c>
@@ -3641,7 +3643,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:18">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -3694,7 +3696,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:18">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -3747,7 +3749,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:18">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -3800,7 +3802,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:18">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -3853,7 +3855,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:18">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -3906,7 +3908,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:18">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -3959,7 +3961,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:18">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -4012,7 +4014,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:18">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -4041,12 +4043,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:18">
       <c r="A67" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="1:18">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -4075,7 +4077,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:18">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -4104,7 +4106,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:18">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -4133,7 +4135,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:18">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -4186,12 +4188,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="1:18">
       <c r="A72" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:18">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -4244,12 +4246,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="1:18">
       <c r="A74" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:18">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:18">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -4355,7 +4357,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="1:18">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -4408,7 +4410,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:18">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -4461,7 +4463,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:18">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -4513,6 +4515,176 @@
       <c r="Q79" t="s">
         <v>96</v>
       </c>
+    </row>
+    <row r="80" spans="1:18">
+      <c r="A80" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" t="s">
+        <v>87</v>
+      </c>
+      <c r="C80" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80" t="s">
+        <v>89</v>
+      </c>
+      <c r="F80" t="s">
+        <v>90</v>
+      </c>
+      <c r="G80" t="s">
+        <v>91</v>
+      </c>
+      <c r="H80" t="s">
+        <v>18</v>
+      </c>
+      <c r="I80" t="s">
+        <v>91</v>
+      </c>
+      <c r="J80" t="s">
+        <v>92</v>
+      </c>
+      <c r="K80" t="s">
+        <v>93</v>
+      </c>
+      <c r="L80" t="s">
+        <v>21</v>
+      </c>
+      <c r="M80" t="s">
+        <v>94</v>
+      </c>
+      <c r="N80" t="s">
+        <v>95</v>
+      </c>
+      <c r="O80" t="s">
+        <v>96</v>
+      </c>
+      <c r="P80" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
+      <c r="A81" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
+      <c r="A82" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>87</v>
+      </c>
+      <c r="C83" t="s">
+        <v>88</v>
+      </c>
+      <c r="D83" t="s">
+        <v>14</v>
+      </c>
+      <c r="E83" t="s">
+        <v>89</v>
+      </c>
+      <c r="F83" t="s">
+        <v>90</v>
+      </c>
+      <c r="G83" t="s">
+        <v>91</v>
+      </c>
+      <c r="H83" t="s">
+        <v>18</v>
+      </c>
+      <c r="I83" t="s">
+        <v>91</v>
+      </c>
+      <c r="J83" t="s">
+        <v>92</v>
+      </c>
+      <c r="K83" t="s">
+        <v>93</v>
+      </c>
+      <c r="L83" t="s">
+        <v>21</v>
+      </c>
+      <c r="M83" t="s">
+        <v>94</v>
+      </c>
+      <c r="N83" t="s">
+        <v>95</v>
+      </c>
+      <c r="O83" t="s">
+        <v>96</v>
+      </c>
+      <c r="P83" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>87</v>
+      </c>
+      <c r="C84" t="s">
+        <v>88</v>
+      </c>
+      <c r="D84" t="s">
+        <v>14</v>
+      </c>
+      <c r="E84" t="s">
+        <v>89</v>
+      </c>
+      <c r="F84" t="s">
+        <v>90</v>
+      </c>
+      <c r="G84" t="s">
+        <v>91</v>
+      </c>
+      <c r="H84" t="s">
+        <v>18</v>
+      </c>
+      <c r="I84" t="s">
+        <v>91</v>
+      </c>
+      <c r="J84" t="s">
+        <v>92</v>
+      </c>
+      <c r="K84" t="s">
+        <v>93</v>
+      </c>
+      <c r="L84" t="s">
+        <v>21</v>
+      </c>
+      <c r="M84" t="s">
+        <v>94</v>
+      </c>
+      <c r="N84" t="s">
+        <v>95</v>
+      </c>
+      <c r="O84" t="s">
+        <v>96</v>
+      </c>
+      <c r="P84" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>96</v>
+      </c>
+      <c r="R84" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4532,7 +4704,7 @@
   </sheetPr>
   <dimension ref="A1:BE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="B5" xSplit="1" ySplit="4"/>
       <selection activeCell="B1" pane="topRight" sqref="B1"/>
       <selection activeCell="A5" pane="bottomLeft" sqref="A5"/>

</xml_diff>

<commit_message>
log_arquivo_ipdo para salvar todas as ações ocorridas durante a execução da rotina arquivo_ipdo
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -6,7 +6,7 @@
     <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet name="Tabela1" sheetId="1" r:id="rId1"/>
+    <s:sheet name="BalancoResumido" sheetId="1" r:id="rId1"/>
     <s:sheet name="BalancoEnergeticoDetalhado" sheetId="2" r:id="rId2"/>
   </s:sheets>
   <s:definedNames/>
@@ -920,10 +920,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4684,7 +4684,60 @@
       <c r="Q84" t="s">
         <v>96</v>
       </c>
-      <c r="R84" t="s"/>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" t="s">
+        <v>87</v>
+      </c>
+      <c r="C85" t="s">
+        <v>88</v>
+      </c>
+      <c r="D85" t="s">
+        <v>14</v>
+      </c>
+      <c r="E85" t="s">
+        <v>89</v>
+      </c>
+      <c r="F85" t="s">
+        <v>90</v>
+      </c>
+      <c r="G85" t="s">
+        <v>91</v>
+      </c>
+      <c r="H85" t="s">
+        <v>18</v>
+      </c>
+      <c r="I85" t="s">
+        <v>91</v>
+      </c>
+      <c r="J85" t="s">
+        <v>92</v>
+      </c>
+      <c r="K85" t="s">
+        <v>93</v>
+      </c>
+      <c r="L85" t="s">
+        <v>21</v>
+      </c>
+      <c r="M85" t="s">
+        <v>94</v>
+      </c>
+      <c r="N85" t="s">
+        <v>95</v>
+      </c>
+      <c r="O85" t="s">
+        <v>96</v>
+      </c>
+      <c r="P85" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>96</v>
+      </c>
+      <c r="R85" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
manipulandos erros  e gerando logs da rotina imprimir_resultados, com a declaração try catch
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -920,7 +920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="E83" sqref="E83"/>
@@ -4737,7 +4737,113 @@
       <c r="Q85" t="s">
         <v>96</v>
       </c>
-      <c r="R85" t="s"/>
+    </row>
+    <row r="86" spans="1:18">
+      <c r="A86" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86" t="s">
+        <v>88</v>
+      </c>
+      <c r="D86" t="s">
+        <v>14</v>
+      </c>
+      <c r="E86" t="s">
+        <v>89</v>
+      </c>
+      <c r="F86" t="s">
+        <v>90</v>
+      </c>
+      <c r="G86" t="s">
+        <v>91</v>
+      </c>
+      <c r="H86" t="s">
+        <v>18</v>
+      </c>
+      <c r="I86" t="s">
+        <v>91</v>
+      </c>
+      <c r="J86" t="s">
+        <v>92</v>
+      </c>
+      <c r="K86" t="s">
+        <v>93</v>
+      </c>
+      <c r="L86" t="s">
+        <v>21</v>
+      </c>
+      <c r="M86" t="s">
+        <v>94</v>
+      </c>
+      <c r="N86" t="s">
+        <v>95</v>
+      </c>
+      <c r="O86" t="s">
+        <v>96</v>
+      </c>
+      <c r="P86" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>87</v>
+      </c>
+      <c r="C87" t="s">
+        <v>88</v>
+      </c>
+      <c r="D87" t="s">
+        <v>14</v>
+      </c>
+      <c r="E87" t="s">
+        <v>89</v>
+      </c>
+      <c r="F87" t="s">
+        <v>90</v>
+      </c>
+      <c r="G87" t="s">
+        <v>91</v>
+      </c>
+      <c r="H87" t="s">
+        <v>18</v>
+      </c>
+      <c r="I87" t="s">
+        <v>91</v>
+      </c>
+      <c r="J87" t="s">
+        <v>92</v>
+      </c>
+      <c r="K87" t="s">
+        <v>93</v>
+      </c>
+      <c r="L87" t="s">
+        <v>21</v>
+      </c>
+      <c r="M87" t="s">
+        <v>94</v>
+      </c>
+      <c r="N87" t="s">
+        <v>95</v>
+      </c>
+      <c r="O87" t="s">
+        <v>96</v>
+      </c>
+      <c r="P87" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>96</v>
+      </c>
+      <c r="R87" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
imprimindo no main linha a linha o json[balanco_detalhado][subsistemas][fontes]
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -920,7 +920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R87"/>
+  <dimension ref="A1:R108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="E83" sqref="E83"/>
@@ -4843,7 +4843,1120 @@
       <c r="Q87" t="s">
         <v>96</v>
       </c>
-      <c r="R87" t="s"/>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>87</v>
+      </c>
+      <c r="C88" t="s">
+        <v>88</v>
+      </c>
+      <c r="D88" t="s">
+        <v>14</v>
+      </c>
+      <c r="E88" t="s">
+        <v>89</v>
+      </c>
+      <c r="F88" t="s">
+        <v>90</v>
+      </c>
+      <c r="G88" t="s">
+        <v>91</v>
+      </c>
+      <c r="H88" t="s">
+        <v>18</v>
+      </c>
+      <c r="I88" t="s">
+        <v>91</v>
+      </c>
+      <c r="J88" t="s">
+        <v>92</v>
+      </c>
+      <c r="K88" t="s">
+        <v>93</v>
+      </c>
+      <c r="L88" t="s">
+        <v>21</v>
+      </c>
+      <c r="M88" t="s">
+        <v>94</v>
+      </c>
+      <c r="N88" t="s">
+        <v>95</v>
+      </c>
+      <c r="O88" t="s">
+        <v>96</v>
+      </c>
+      <c r="P88" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
+      <c r="A89" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" t="s">
+        <v>87</v>
+      </c>
+      <c r="C89" t="s">
+        <v>88</v>
+      </c>
+      <c r="D89" t="s">
+        <v>14</v>
+      </c>
+      <c r="E89" t="s">
+        <v>89</v>
+      </c>
+      <c r="F89" t="s">
+        <v>90</v>
+      </c>
+      <c r="G89" t="s">
+        <v>91</v>
+      </c>
+      <c r="H89" t="s">
+        <v>18</v>
+      </c>
+      <c r="I89" t="s">
+        <v>91</v>
+      </c>
+      <c r="J89" t="s">
+        <v>92</v>
+      </c>
+      <c r="K89" t="s">
+        <v>93</v>
+      </c>
+      <c r="L89" t="s">
+        <v>21</v>
+      </c>
+      <c r="M89" t="s">
+        <v>94</v>
+      </c>
+      <c r="N89" t="s">
+        <v>95</v>
+      </c>
+      <c r="O89" t="s">
+        <v>96</v>
+      </c>
+      <c r="P89" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
+      <c r="A90" t="s">
+        <v>86</v>
+      </c>
+      <c r="B90" t="s">
+        <v>87</v>
+      </c>
+      <c r="C90" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90" t="s">
+        <v>14</v>
+      </c>
+      <c r="E90" t="s">
+        <v>89</v>
+      </c>
+      <c r="F90" t="s">
+        <v>90</v>
+      </c>
+      <c r="G90" t="s">
+        <v>91</v>
+      </c>
+      <c r="H90" t="s">
+        <v>18</v>
+      </c>
+      <c r="I90" t="s">
+        <v>91</v>
+      </c>
+      <c r="J90" t="s">
+        <v>92</v>
+      </c>
+      <c r="K90" t="s">
+        <v>93</v>
+      </c>
+      <c r="L90" t="s">
+        <v>21</v>
+      </c>
+      <c r="M90" t="s">
+        <v>94</v>
+      </c>
+      <c r="N90" t="s">
+        <v>95</v>
+      </c>
+      <c r="O90" t="s">
+        <v>96</v>
+      </c>
+      <c r="P90" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18">
+      <c r="A91" t="s">
+        <v>86</v>
+      </c>
+      <c r="B91" t="s">
+        <v>87</v>
+      </c>
+      <c r="C91" t="s">
+        <v>88</v>
+      </c>
+      <c r="D91" t="s">
+        <v>14</v>
+      </c>
+      <c r="E91" t="s">
+        <v>89</v>
+      </c>
+      <c r="F91" t="s">
+        <v>90</v>
+      </c>
+      <c r="G91" t="s">
+        <v>91</v>
+      </c>
+      <c r="H91" t="s">
+        <v>18</v>
+      </c>
+      <c r="I91" t="s">
+        <v>91</v>
+      </c>
+      <c r="J91" t="s">
+        <v>92</v>
+      </c>
+      <c r="K91" t="s">
+        <v>93</v>
+      </c>
+      <c r="L91" t="s">
+        <v>21</v>
+      </c>
+      <c r="M91" t="s">
+        <v>94</v>
+      </c>
+      <c r="N91" t="s">
+        <v>95</v>
+      </c>
+      <c r="O91" t="s">
+        <v>96</v>
+      </c>
+      <c r="P91" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18">
+      <c r="A92" t="s">
+        <v>86</v>
+      </c>
+      <c r="B92" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" t="s">
+        <v>88</v>
+      </c>
+      <c r="D92" t="s">
+        <v>14</v>
+      </c>
+      <c r="E92" t="s">
+        <v>89</v>
+      </c>
+      <c r="F92" t="s">
+        <v>90</v>
+      </c>
+      <c r="G92" t="s">
+        <v>91</v>
+      </c>
+      <c r="H92" t="s">
+        <v>18</v>
+      </c>
+      <c r="I92" t="s">
+        <v>91</v>
+      </c>
+      <c r="J92" t="s">
+        <v>92</v>
+      </c>
+      <c r="K92" t="s">
+        <v>93</v>
+      </c>
+      <c r="L92" t="s">
+        <v>21</v>
+      </c>
+      <c r="M92" t="s">
+        <v>94</v>
+      </c>
+      <c r="N92" t="s">
+        <v>95</v>
+      </c>
+      <c r="O92" t="s">
+        <v>96</v>
+      </c>
+      <c r="P92" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18">
+      <c r="A93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B93" t="s">
+        <v>87</v>
+      </c>
+      <c r="C93" t="s">
+        <v>88</v>
+      </c>
+      <c r="D93" t="s">
+        <v>14</v>
+      </c>
+      <c r="E93" t="s">
+        <v>89</v>
+      </c>
+      <c r="F93" t="s">
+        <v>90</v>
+      </c>
+      <c r="G93" t="s">
+        <v>91</v>
+      </c>
+      <c r="H93" t="s">
+        <v>18</v>
+      </c>
+      <c r="I93" t="s">
+        <v>91</v>
+      </c>
+      <c r="J93" t="s">
+        <v>92</v>
+      </c>
+      <c r="K93" t="s">
+        <v>93</v>
+      </c>
+      <c r="L93" t="s">
+        <v>21</v>
+      </c>
+      <c r="M93" t="s">
+        <v>94</v>
+      </c>
+      <c r="N93" t="s">
+        <v>95</v>
+      </c>
+      <c r="O93" t="s">
+        <v>96</v>
+      </c>
+      <c r="P93" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18">
+      <c r="A94" t="s">
+        <v>86</v>
+      </c>
+      <c r="B94" t="s">
+        <v>87</v>
+      </c>
+      <c r="C94" t="s">
+        <v>88</v>
+      </c>
+      <c r="D94" t="s">
+        <v>14</v>
+      </c>
+      <c r="E94" t="s">
+        <v>89</v>
+      </c>
+      <c r="F94" t="s">
+        <v>90</v>
+      </c>
+      <c r="G94" t="s">
+        <v>91</v>
+      </c>
+      <c r="H94" t="s">
+        <v>18</v>
+      </c>
+      <c r="I94" t="s">
+        <v>91</v>
+      </c>
+      <c r="J94" t="s">
+        <v>92</v>
+      </c>
+      <c r="K94" t="s">
+        <v>93</v>
+      </c>
+      <c r="L94" t="s">
+        <v>21</v>
+      </c>
+      <c r="M94" t="s">
+        <v>94</v>
+      </c>
+      <c r="N94" t="s">
+        <v>95</v>
+      </c>
+      <c r="O94" t="s">
+        <v>96</v>
+      </c>
+      <c r="P94" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18">
+      <c r="A95" t="s">
+        <v>86</v>
+      </c>
+      <c r="B95" t="s">
+        <v>87</v>
+      </c>
+      <c r="C95" t="s">
+        <v>88</v>
+      </c>
+      <c r="D95" t="s">
+        <v>14</v>
+      </c>
+      <c r="E95" t="s">
+        <v>89</v>
+      </c>
+      <c r="F95" t="s">
+        <v>90</v>
+      </c>
+      <c r="G95" t="s">
+        <v>91</v>
+      </c>
+      <c r="H95" t="s">
+        <v>18</v>
+      </c>
+      <c r="I95" t="s">
+        <v>91</v>
+      </c>
+      <c r="J95" t="s">
+        <v>92</v>
+      </c>
+      <c r="K95" t="s">
+        <v>93</v>
+      </c>
+      <c r="L95" t="s">
+        <v>21</v>
+      </c>
+      <c r="M95" t="s">
+        <v>94</v>
+      </c>
+      <c r="N95" t="s">
+        <v>95</v>
+      </c>
+      <c r="O95" t="s">
+        <v>96</v>
+      </c>
+      <c r="P95" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18">
+      <c r="A96" t="s">
+        <v>86</v>
+      </c>
+      <c r="B96" t="s">
+        <v>87</v>
+      </c>
+      <c r="C96" t="s">
+        <v>88</v>
+      </c>
+      <c r="D96" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" t="s">
+        <v>89</v>
+      </c>
+      <c r="F96" t="s">
+        <v>90</v>
+      </c>
+      <c r="G96" t="s">
+        <v>91</v>
+      </c>
+      <c r="H96" t="s">
+        <v>18</v>
+      </c>
+      <c r="I96" t="s">
+        <v>91</v>
+      </c>
+      <c r="J96" t="s">
+        <v>92</v>
+      </c>
+      <c r="K96" t="s">
+        <v>93</v>
+      </c>
+      <c r="L96" t="s">
+        <v>21</v>
+      </c>
+      <c r="M96" t="s">
+        <v>94</v>
+      </c>
+      <c r="N96" t="s">
+        <v>95</v>
+      </c>
+      <c r="O96" t="s">
+        <v>96</v>
+      </c>
+      <c r="P96" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18">
+      <c r="A97" t="s">
+        <v>86</v>
+      </c>
+      <c r="B97" t="s">
+        <v>87</v>
+      </c>
+      <c r="C97" t="s">
+        <v>88</v>
+      </c>
+      <c r="D97" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" t="s">
+        <v>89</v>
+      </c>
+      <c r="F97" t="s">
+        <v>90</v>
+      </c>
+      <c r="G97" t="s">
+        <v>91</v>
+      </c>
+      <c r="H97" t="s">
+        <v>18</v>
+      </c>
+      <c r="I97" t="s">
+        <v>91</v>
+      </c>
+      <c r="J97" t="s">
+        <v>92</v>
+      </c>
+      <c r="K97" t="s">
+        <v>93</v>
+      </c>
+      <c r="L97" t="s">
+        <v>21</v>
+      </c>
+      <c r="M97" t="s">
+        <v>94</v>
+      </c>
+      <c r="N97" t="s">
+        <v>95</v>
+      </c>
+      <c r="O97" t="s">
+        <v>96</v>
+      </c>
+      <c r="P97" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18">
+      <c r="A98" t="s">
+        <v>86</v>
+      </c>
+      <c r="B98" t="s">
+        <v>87</v>
+      </c>
+      <c r="C98" t="s">
+        <v>88</v>
+      </c>
+      <c r="D98" t="s">
+        <v>14</v>
+      </c>
+      <c r="E98" t="s">
+        <v>89</v>
+      </c>
+      <c r="F98" t="s">
+        <v>90</v>
+      </c>
+      <c r="G98" t="s">
+        <v>91</v>
+      </c>
+      <c r="H98" t="s">
+        <v>18</v>
+      </c>
+      <c r="I98" t="s">
+        <v>91</v>
+      </c>
+      <c r="J98" t="s">
+        <v>92</v>
+      </c>
+      <c r="K98" t="s">
+        <v>93</v>
+      </c>
+      <c r="L98" t="s">
+        <v>21</v>
+      </c>
+      <c r="M98" t="s">
+        <v>94</v>
+      </c>
+      <c r="N98" t="s">
+        <v>95</v>
+      </c>
+      <c r="O98" t="s">
+        <v>96</v>
+      </c>
+      <c r="P98" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18">
+      <c r="A99" t="s">
+        <v>86</v>
+      </c>
+      <c r="B99" t="s">
+        <v>87</v>
+      </c>
+      <c r="C99" t="s">
+        <v>88</v>
+      </c>
+      <c r="D99" t="s">
+        <v>14</v>
+      </c>
+      <c r="E99" t="s">
+        <v>89</v>
+      </c>
+      <c r="F99" t="s">
+        <v>90</v>
+      </c>
+      <c r="G99" t="s">
+        <v>91</v>
+      </c>
+      <c r="H99" t="s">
+        <v>18</v>
+      </c>
+      <c r="I99" t="s">
+        <v>91</v>
+      </c>
+      <c r="J99" t="s">
+        <v>92</v>
+      </c>
+      <c r="K99" t="s">
+        <v>93</v>
+      </c>
+      <c r="L99" t="s">
+        <v>21</v>
+      </c>
+      <c r="M99" t="s">
+        <v>94</v>
+      </c>
+      <c r="N99" t="s">
+        <v>95</v>
+      </c>
+      <c r="O99" t="s">
+        <v>96</v>
+      </c>
+      <c r="P99" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" t="s">
+        <v>87</v>
+      </c>
+      <c r="C100" t="s">
+        <v>88</v>
+      </c>
+      <c r="D100" t="s">
+        <v>14</v>
+      </c>
+      <c r="E100" t="s">
+        <v>89</v>
+      </c>
+      <c r="F100" t="s">
+        <v>90</v>
+      </c>
+      <c r="G100" t="s">
+        <v>91</v>
+      </c>
+      <c r="H100" t="s">
+        <v>18</v>
+      </c>
+      <c r="I100" t="s">
+        <v>91</v>
+      </c>
+      <c r="J100" t="s">
+        <v>92</v>
+      </c>
+      <c r="K100" t="s">
+        <v>93</v>
+      </c>
+      <c r="L100" t="s">
+        <v>21</v>
+      </c>
+      <c r="M100" t="s">
+        <v>94</v>
+      </c>
+      <c r="N100" t="s">
+        <v>95</v>
+      </c>
+      <c r="O100" t="s">
+        <v>96</v>
+      </c>
+      <c r="P100" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18">
+      <c r="A101" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" t="s">
+        <v>87</v>
+      </c>
+      <c r="C101" t="s">
+        <v>88</v>
+      </c>
+      <c r="D101" t="s">
+        <v>14</v>
+      </c>
+      <c r="E101" t="s">
+        <v>89</v>
+      </c>
+      <c r="F101" t="s">
+        <v>90</v>
+      </c>
+      <c r="G101" t="s">
+        <v>91</v>
+      </c>
+      <c r="H101" t="s">
+        <v>18</v>
+      </c>
+      <c r="I101" t="s">
+        <v>91</v>
+      </c>
+      <c r="J101" t="s">
+        <v>92</v>
+      </c>
+      <c r="K101" t="s">
+        <v>93</v>
+      </c>
+      <c r="L101" t="s">
+        <v>21</v>
+      </c>
+      <c r="M101" t="s">
+        <v>94</v>
+      </c>
+      <c r="N101" t="s">
+        <v>95</v>
+      </c>
+      <c r="O101" t="s">
+        <v>96</v>
+      </c>
+      <c r="P101" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18">
+      <c r="A102" t="s">
+        <v>86</v>
+      </c>
+      <c r="B102" t="s">
+        <v>87</v>
+      </c>
+      <c r="C102" t="s">
+        <v>88</v>
+      </c>
+      <c r="D102" t="s">
+        <v>14</v>
+      </c>
+      <c r="E102" t="s">
+        <v>89</v>
+      </c>
+      <c r="F102" t="s">
+        <v>90</v>
+      </c>
+      <c r="G102" t="s">
+        <v>91</v>
+      </c>
+      <c r="H102" t="s">
+        <v>18</v>
+      </c>
+      <c r="I102" t="s">
+        <v>91</v>
+      </c>
+      <c r="J102" t="s">
+        <v>92</v>
+      </c>
+      <c r="K102" t="s">
+        <v>93</v>
+      </c>
+      <c r="L102" t="s">
+        <v>21</v>
+      </c>
+      <c r="M102" t="s">
+        <v>94</v>
+      </c>
+      <c r="N102" t="s">
+        <v>95</v>
+      </c>
+      <c r="O102" t="s">
+        <v>96</v>
+      </c>
+      <c r="P102" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18">
+      <c r="A103" t="s">
+        <v>86</v>
+      </c>
+      <c r="B103" t="s">
+        <v>87</v>
+      </c>
+      <c r="C103" t="s">
+        <v>88</v>
+      </c>
+      <c r="D103" t="s">
+        <v>14</v>
+      </c>
+      <c r="E103" t="s">
+        <v>89</v>
+      </c>
+      <c r="F103" t="s">
+        <v>90</v>
+      </c>
+      <c r="G103" t="s">
+        <v>91</v>
+      </c>
+      <c r="H103" t="s">
+        <v>18</v>
+      </c>
+      <c r="I103" t="s">
+        <v>91</v>
+      </c>
+      <c r="J103" t="s">
+        <v>92</v>
+      </c>
+      <c r="K103" t="s">
+        <v>93</v>
+      </c>
+      <c r="L103" t="s">
+        <v>21</v>
+      </c>
+      <c r="M103" t="s">
+        <v>94</v>
+      </c>
+      <c r="N103" t="s">
+        <v>95</v>
+      </c>
+      <c r="O103" t="s">
+        <v>96</v>
+      </c>
+      <c r="P103" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18">
+      <c r="A104" t="s">
+        <v>86</v>
+      </c>
+      <c r="B104" t="s">
+        <v>87</v>
+      </c>
+      <c r="C104" t="s">
+        <v>88</v>
+      </c>
+      <c r="D104" t="s">
+        <v>14</v>
+      </c>
+      <c r="E104" t="s">
+        <v>89</v>
+      </c>
+      <c r="F104" t="s">
+        <v>90</v>
+      </c>
+      <c r="G104" t="s">
+        <v>91</v>
+      </c>
+      <c r="H104" t="s">
+        <v>18</v>
+      </c>
+      <c r="I104" t="s">
+        <v>91</v>
+      </c>
+      <c r="J104" t="s">
+        <v>92</v>
+      </c>
+      <c r="K104" t="s">
+        <v>93</v>
+      </c>
+      <c r="L104" t="s">
+        <v>21</v>
+      </c>
+      <c r="M104" t="s">
+        <v>94</v>
+      </c>
+      <c r="N104" t="s">
+        <v>95</v>
+      </c>
+      <c r="O104" t="s">
+        <v>96</v>
+      </c>
+      <c r="P104" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18">
+      <c r="A105" t="s">
+        <v>86</v>
+      </c>
+      <c r="B105" t="s">
+        <v>87</v>
+      </c>
+      <c r="C105" t="s">
+        <v>88</v>
+      </c>
+      <c r="D105" t="s">
+        <v>14</v>
+      </c>
+      <c r="E105" t="s">
+        <v>89</v>
+      </c>
+      <c r="F105" t="s">
+        <v>90</v>
+      </c>
+      <c r="G105" t="s">
+        <v>91</v>
+      </c>
+      <c r="H105" t="s">
+        <v>18</v>
+      </c>
+      <c r="I105" t="s">
+        <v>91</v>
+      </c>
+      <c r="J105" t="s">
+        <v>92</v>
+      </c>
+      <c r="K105" t="s">
+        <v>93</v>
+      </c>
+      <c r="L105" t="s">
+        <v>21</v>
+      </c>
+      <c r="M105" t="s">
+        <v>94</v>
+      </c>
+      <c r="N105" t="s">
+        <v>95</v>
+      </c>
+      <c r="O105" t="s">
+        <v>96</v>
+      </c>
+      <c r="P105" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18">
+      <c r="A106" t="s">
+        <v>86</v>
+      </c>
+      <c r="B106" t="s">
+        <v>87</v>
+      </c>
+      <c r="C106" t="s">
+        <v>88</v>
+      </c>
+      <c r="D106" t="s">
+        <v>14</v>
+      </c>
+      <c r="E106" t="s">
+        <v>89</v>
+      </c>
+      <c r="F106" t="s">
+        <v>90</v>
+      </c>
+      <c r="G106" t="s">
+        <v>91</v>
+      </c>
+      <c r="H106" t="s">
+        <v>18</v>
+      </c>
+      <c r="I106" t="s">
+        <v>91</v>
+      </c>
+      <c r="J106" t="s">
+        <v>92</v>
+      </c>
+      <c r="K106" t="s">
+        <v>93</v>
+      </c>
+      <c r="L106" t="s">
+        <v>21</v>
+      </c>
+      <c r="M106" t="s">
+        <v>94</v>
+      </c>
+      <c r="N106" t="s">
+        <v>95</v>
+      </c>
+      <c r="O106" t="s">
+        <v>96</v>
+      </c>
+      <c r="P106" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18">
+      <c r="A107" t="s">
+        <v>86</v>
+      </c>
+      <c r="B107" t="s">
+        <v>87</v>
+      </c>
+      <c r="C107" t="s">
+        <v>88</v>
+      </c>
+      <c r="D107" t="s">
+        <v>14</v>
+      </c>
+      <c r="E107" t="s">
+        <v>89</v>
+      </c>
+      <c r="F107" t="s">
+        <v>90</v>
+      </c>
+      <c r="G107" t="s">
+        <v>91</v>
+      </c>
+      <c r="H107" t="s">
+        <v>18</v>
+      </c>
+      <c r="I107" t="s">
+        <v>91</v>
+      </c>
+      <c r="J107" t="s">
+        <v>92</v>
+      </c>
+      <c r="K107" t="s">
+        <v>93</v>
+      </c>
+      <c r="L107" t="s">
+        <v>21</v>
+      </c>
+      <c r="M107" t="s">
+        <v>94</v>
+      </c>
+      <c r="N107" t="s">
+        <v>95</v>
+      </c>
+      <c r="O107" t="s">
+        <v>96</v>
+      </c>
+      <c r="P107" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18">
+      <c r="A108" t="s">
+        <v>86</v>
+      </c>
+      <c r="B108" t="s">
+        <v>87</v>
+      </c>
+      <c r="C108" t="s">
+        <v>88</v>
+      </c>
+      <c r="D108" t="s">
+        <v>14</v>
+      </c>
+      <c r="E108" t="s">
+        <v>89</v>
+      </c>
+      <c r="F108" t="s">
+        <v>90</v>
+      </c>
+      <c r="G108" t="s">
+        <v>91</v>
+      </c>
+      <c r="H108" t="s">
+        <v>18</v>
+      </c>
+      <c r="I108" t="s">
+        <v>91</v>
+      </c>
+      <c r="J108" t="s">
+        <v>92</v>
+      </c>
+      <c r="K108" t="s">
+        <v>93</v>
+      </c>
+      <c r="L108" t="s">
+        <v>21</v>
+      </c>
+      <c r="M108" t="s">
+        <v>94</v>
+      </c>
+      <c r="N108" t="s">
+        <v>95</v>
+      </c>
+      <c r="O108" t="s">
+        <v>96</v>
+      </c>
+      <c r="P108" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>96</v>
+      </c>
+      <c r="R108" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
prettify json e substitui Termo (**) por Termo no tratamento de strings das fontes energéticas
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -920,7 +920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R108"/>
+  <dimension ref="A1:R111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="E83" sqref="E83"/>
@@ -5956,7 +5956,166 @@
       <c r="Q108" t="s">
         <v>96</v>
       </c>
-      <c r="R108" t="s"/>
+    </row>
+    <row r="109" spans="1:18">
+      <c r="A109" t="s">
+        <v>86</v>
+      </c>
+      <c r="B109" t="s">
+        <v>87</v>
+      </c>
+      <c r="C109" t="s">
+        <v>88</v>
+      </c>
+      <c r="D109" t="s">
+        <v>14</v>
+      </c>
+      <c r="E109" t="s">
+        <v>89</v>
+      </c>
+      <c r="F109" t="s">
+        <v>90</v>
+      </c>
+      <c r="G109" t="s">
+        <v>91</v>
+      </c>
+      <c r="H109" t="s">
+        <v>18</v>
+      </c>
+      <c r="I109" t="s">
+        <v>91</v>
+      </c>
+      <c r="J109" t="s">
+        <v>92</v>
+      </c>
+      <c r="K109" t="s">
+        <v>93</v>
+      </c>
+      <c r="L109" t="s">
+        <v>21</v>
+      </c>
+      <c r="M109" t="s">
+        <v>94</v>
+      </c>
+      <c r="N109" t="s">
+        <v>95</v>
+      </c>
+      <c r="O109" t="s">
+        <v>96</v>
+      </c>
+      <c r="P109" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18">
+      <c r="A110" t="s">
+        <v>86</v>
+      </c>
+      <c r="B110" t="s">
+        <v>87</v>
+      </c>
+      <c r="C110" t="s">
+        <v>88</v>
+      </c>
+      <c r="D110" t="s">
+        <v>14</v>
+      </c>
+      <c r="E110" t="s">
+        <v>89</v>
+      </c>
+      <c r="F110" t="s">
+        <v>90</v>
+      </c>
+      <c r="G110" t="s">
+        <v>91</v>
+      </c>
+      <c r="H110" t="s">
+        <v>18</v>
+      </c>
+      <c r="I110" t="s">
+        <v>91</v>
+      </c>
+      <c r="J110" t="s">
+        <v>92</v>
+      </c>
+      <c r="K110" t="s">
+        <v>93</v>
+      </c>
+      <c r="L110" t="s">
+        <v>21</v>
+      </c>
+      <c r="M110" t="s">
+        <v>94</v>
+      </c>
+      <c r="N110" t="s">
+        <v>95</v>
+      </c>
+      <c r="O110" t="s">
+        <v>96</v>
+      </c>
+      <c r="P110" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18">
+      <c r="A111" t="s">
+        <v>86</v>
+      </c>
+      <c r="B111" t="s">
+        <v>87</v>
+      </c>
+      <c r="C111" t="s">
+        <v>88</v>
+      </c>
+      <c r="D111" t="s">
+        <v>14</v>
+      </c>
+      <c r="E111" t="s">
+        <v>89</v>
+      </c>
+      <c r="F111" t="s">
+        <v>90</v>
+      </c>
+      <c r="G111" t="s">
+        <v>91</v>
+      </c>
+      <c r="H111" t="s">
+        <v>18</v>
+      </c>
+      <c r="I111" t="s">
+        <v>91</v>
+      </c>
+      <c r="J111" t="s">
+        <v>92</v>
+      </c>
+      <c r="K111" t="s">
+        <v>93</v>
+      </c>
+      <c r="L111" t="s">
+        <v>21</v>
+      </c>
+      <c r="M111" t="s">
+        <v>94</v>
+      </c>
+      <c r="N111" t="s">
+        <v>95</v>
+      </c>
+      <c r="O111" t="s">
+        <v>96</v>
+      </c>
+      <c r="P111" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>96</v>
+      </c>
+      <c r="R111" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
estrutura para imprimir o balanço_detalhado_em_xlsx
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -3863,7 +3863,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R302"/>
+  <dimension ref="A1:R310"/>
   <sheetViews>
     <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="A116" sqref="A116"/>
@@ -19181,7 +19181,431 @@
       <c r="Q302" t="s">
         <v>829</v>
       </c>
-      <c r="R302" t="s"/>
+    </row>
+    <row r="303" spans="1:18">
+      <c r="A303" t="s">
+        <v>368</v>
+      </c>
+      <c r="B303" t="s">
+        <v>369</v>
+      </c>
+      <c r="C303" t="s">
+        <v>370</v>
+      </c>
+      <c r="D303" t="s">
+        <v>14</v>
+      </c>
+      <c r="E303" t="s">
+        <v>371</v>
+      </c>
+      <c r="F303" t="s">
+        <v>372</v>
+      </c>
+      <c r="G303" t="s">
+        <v>373</v>
+      </c>
+      <c r="H303" t="s">
+        <v>374</v>
+      </c>
+      <c r="I303" t="s">
+        <v>375</v>
+      </c>
+      <c r="J303" t="s">
+        <v>376</v>
+      </c>
+      <c r="K303" t="s">
+        <v>377</v>
+      </c>
+      <c r="L303" t="s">
+        <v>44</v>
+      </c>
+      <c r="M303" t="s">
+        <v>378</v>
+      </c>
+      <c r="N303" t="s">
+        <v>379</v>
+      </c>
+      <c r="O303" t="s">
+        <v>380</v>
+      </c>
+      <c r="P303" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q303" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="304" spans="1:18">
+      <c r="A304" t="s">
+        <v>383</v>
+      </c>
+      <c r="B304" t="s">
+        <v>384</v>
+      </c>
+      <c r="C304" t="s">
+        <v>355</v>
+      </c>
+      <c r="D304" t="s">
+        <v>14</v>
+      </c>
+      <c r="E304" t="s">
+        <v>385</v>
+      </c>
+      <c r="F304" t="s">
+        <v>386</v>
+      </c>
+      <c r="G304" t="s">
+        <v>387</v>
+      </c>
+      <c r="H304" t="s">
+        <v>388</v>
+      </c>
+      <c r="I304" t="s">
+        <v>389</v>
+      </c>
+      <c r="J304" t="s">
+        <v>390</v>
+      </c>
+      <c r="K304" t="s">
+        <v>391</v>
+      </c>
+      <c r="L304" t="s">
+        <v>106</v>
+      </c>
+      <c r="M304" t="s">
+        <v>392</v>
+      </c>
+      <c r="N304" t="s">
+        <v>393</v>
+      </c>
+      <c r="O304" t="s">
+        <v>394</v>
+      </c>
+      <c r="P304" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q304" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="305" spans="1:18">
+      <c r="A305" t="s">
+        <v>397</v>
+      </c>
+      <c r="B305" t="s">
+        <v>398</v>
+      </c>
+      <c r="C305" t="s">
+        <v>399</v>
+      </c>
+      <c r="D305" t="s">
+        <v>14</v>
+      </c>
+      <c r="E305" t="s">
+        <v>400</v>
+      </c>
+      <c r="F305" t="s">
+        <v>401</v>
+      </c>
+      <c r="G305" t="s">
+        <v>402</v>
+      </c>
+      <c r="H305" t="s">
+        <v>18</v>
+      </c>
+      <c r="I305" t="s">
+        <v>402</v>
+      </c>
+      <c r="J305" t="s">
+        <v>403</v>
+      </c>
+      <c r="K305" t="s">
+        <v>404</v>
+      </c>
+      <c r="L305" t="s">
+        <v>106</v>
+      </c>
+      <c r="M305" t="s">
+        <v>405</v>
+      </c>
+      <c r="N305" t="s">
+        <v>406</v>
+      </c>
+      <c r="O305" t="s">
+        <v>407</v>
+      </c>
+      <c r="P305" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q305" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="306" spans="1:18">
+      <c r="A306" t="s">
+        <v>368</v>
+      </c>
+      <c r="B306" t="s">
+        <v>369</v>
+      </c>
+      <c r="C306" t="s">
+        <v>370</v>
+      </c>
+      <c r="D306" t="s">
+        <v>14</v>
+      </c>
+      <c r="E306" t="s">
+        <v>371</v>
+      </c>
+      <c r="F306" t="s">
+        <v>372</v>
+      </c>
+      <c r="G306" t="s">
+        <v>373</v>
+      </c>
+      <c r="H306" t="s">
+        <v>374</v>
+      </c>
+      <c r="I306" t="s">
+        <v>375</v>
+      </c>
+      <c r="J306" t="s">
+        <v>376</v>
+      </c>
+      <c r="K306" t="s">
+        <v>377</v>
+      </c>
+      <c r="L306" t="s">
+        <v>44</v>
+      </c>
+      <c r="M306" t="s">
+        <v>378</v>
+      </c>
+      <c r="N306" t="s">
+        <v>379</v>
+      </c>
+      <c r="O306" t="s">
+        <v>380</v>
+      </c>
+      <c r="P306" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q306" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="307" spans="1:18">
+      <c r="A307" t="s">
+        <v>383</v>
+      </c>
+      <c r="B307" t="s">
+        <v>384</v>
+      </c>
+      <c r="C307" t="s">
+        <v>355</v>
+      </c>
+      <c r="D307" t="s">
+        <v>14</v>
+      </c>
+      <c r="E307" t="s">
+        <v>385</v>
+      </c>
+      <c r="F307" t="s">
+        <v>386</v>
+      </c>
+      <c r="G307" t="s">
+        <v>387</v>
+      </c>
+      <c r="H307" t="s">
+        <v>388</v>
+      </c>
+      <c r="I307" t="s">
+        <v>389</v>
+      </c>
+      <c r="J307" t="s">
+        <v>390</v>
+      </c>
+      <c r="K307" t="s">
+        <v>391</v>
+      </c>
+      <c r="L307" t="s">
+        <v>106</v>
+      </c>
+      <c r="M307" t="s">
+        <v>392</v>
+      </c>
+      <c r="N307" t="s">
+        <v>393</v>
+      </c>
+      <c r="O307" t="s">
+        <v>394</v>
+      </c>
+      <c r="P307" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q307" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="308" spans="1:18">
+      <c r="A308" t="s">
+        <v>368</v>
+      </c>
+      <c r="B308" t="s">
+        <v>369</v>
+      </c>
+      <c r="C308" t="s">
+        <v>370</v>
+      </c>
+      <c r="D308" t="s">
+        <v>14</v>
+      </c>
+      <c r="E308" t="s">
+        <v>371</v>
+      </c>
+      <c r="F308" t="s">
+        <v>372</v>
+      </c>
+      <c r="G308" t="s">
+        <v>373</v>
+      </c>
+      <c r="H308" t="s">
+        <v>374</v>
+      </c>
+      <c r="I308" t="s">
+        <v>375</v>
+      </c>
+      <c r="J308" t="s">
+        <v>376</v>
+      </c>
+      <c r="K308" t="s">
+        <v>377</v>
+      </c>
+      <c r="L308" t="s">
+        <v>44</v>
+      </c>
+      <c r="M308" t="s">
+        <v>378</v>
+      </c>
+      <c r="N308" t="s">
+        <v>379</v>
+      </c>
+      <c r="O308" t="s">
+        <v>380</v>
+      </c>
+      <c r="P308" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q308" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="309" spans="1:18">
+      <c r="A309" t="s">
+        <v>383</v>
+      </c>
+      <c r="B309" t="s">
+        <v>384</v>
+      </c>
+      <c r="C309" t="s">
+        <v>355</v>
+      </c>
+      <c r="D309" t="s">
+        <v>14</v>
+      </c>
+      <c r="E309" t="s">
+        <v>385</v>
+      </c>
+      <c r="F309" t="s">
+        <v>386</v>
+      </c>
+      <c r="G309" t="s">
+        <v>387</v>
+      </c>
+      <c r="H309" t="s">
+        <v>388</v>
+      </c>
+      <c r="I309" t="s">
+        <v>389</v>
+      </c>
+      <c r="J309" t="s">
+        <v>390</v>
+      </c>
+      <c r="K309" t="s">
+        <v>391</v>
+      </c>
+      <c r="L309" t="s">
+        <v>106</v>
+      </c>
+      <c r="M309" t="s">
+        <v>392</v>
+      </c>
+      <c r="N309" t="s">
+        <v>393</v>
+      </c>
+      <c r="O309" t="s">
+        <v>394</v>
+      </c>
+      <c r="P309" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q309" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="310" spans="1:18">
+      <c r="A310" t="s">
+        <v>368</v>
+      </c>
+      <c r="B310" t="s">
+        <v>369</v>
+      </c>
+      <c r="C310" t="s">
+        <v>370</v>
+      </c>
+      <c r="D310" t="s">
+        <v>14</v>
+      </c>
+      <c r="E310" t="s">
+        <v>371</v>
+      </c>
+      <c r="F310" t="s">
+        <v>372</v>
+      </c>
+      <c r="G310" t="s">
+        <v>373</v>
+      </c>
+      <c r="H310" t="s">
+        <v>374</v>
+      </c>
+      <c r="I310" t="s">
+        <v>375</v>
+      </c>
+      <c r="J310" t="s">
+        <v>376</v>
+      </c>
+      <c r="K310" t="s">
+        <v>377</v>
+      </c>
+      <c r="L310" t="s">
+        <v>44</v>
+      </c>
+      <c r="M310" t="s">
+        <v>378</v>
+      </c>
+      <c r="N310" t="s">
+        <v>379</v>
+      </c>
+      <c r="O310" t="s">
+        <v>380</v>
+      </c>
+      <c r="P310" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q310" t="s">
+        <v>382</v>
+      </c>
+      <c r="R310" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
zerando todas as células do arquivo de saída do balanço energético detalhado
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -1991,7 +1991,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:R40"/>
+  <dimension ref="A3:R70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A355" sqref="A5:Q355"/>
@@ -3990,6 +3990,1596 @@
         <v>394</v>
       </c>
     </row>
+    <row r="41" spans="1:18">
+      <c r="A41" t="s">
+        <v>384</v>
+      </c>
+      <c r="B41" t="s">
+        <v>385</v>
+      </c>
+      <c r="C41" t="s">
+        <v>386</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>387</v>
+      </c>
+      <c r="F41" t="s">
+        <v>388</v>
+      </c>
+      <c r="G41" t="s">
+        <v>389</v>
+      </c>
+      <c r="H41" t="s">
+        <v>50</v>
+      </c>
+      <c r="I41" t="s">
+        <v>389</v>
+      </c>
+      <c r="J41" t="s">
+        <v>390</v>
+      </c>
+      <c r="K41" t="s">
+        <v>391</v>
+      </c>
+      <c r="L41" t="s">
+        <v>75</v>
+      </c>
+      <c r="M41" t="s">
+        <v>392</v>
+      </c>
+      <c r="N41" t="s">
+        <v>393</v>
+      </c>
+      <c r="O41" t="s">
+        <v>394</v>
+      </c>
+      <c r="P41" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" t="s">
+        <v>384</v>
+      </c>
+      <c r="B42" t="s">
+        <v>385</v>
+      </c>
+      <c r="C42" t="s">
+        <v>386</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>387</v>
+      </c>
+      <c r="F42" t="s">
+        <v>388</v>
+      </c>
+      <c r="G42" t="s">
+        <v>389</v>
+      </c>
+      <c r="H42" t="s">
+        <v>50</v>
+      </c>
+      <c r="I42" t="s">
+        <v>389</v>
+      </c>
+      <c r="J42" t="s">
+        <v>390</v>
+      </c>
+      <c r="K42" t="s">
+        <v>391</v>
+      </c>
+      <c r="L42" t="s">
+        <v>75</v>
+      </c>
+      <c r="M42" t="s">
+        <v>392</v>
+      </c>
+      <c r="N42" t="s">
+        <v>393</v>
+      </c>
+      <c r="O42" t="s">
+        <v>394</v>
+      </c>
+      <c r="P42" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" t="s">
+        <v>384</v>
+      </c>
+      <c r="B43" t="s">
+        <v>385</v>
+      </c>
+      <c r="C43" t="s">
+        <v>386</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>387</v>
+      </c>
+      <c r="F43" t="s">
+        <v>388</v>
+      </c>
+      <c r="G43" t="s">
+        <v>389</v>
+      </c>
+      <c r="H43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43" t="s">
+        <v>389</v>
+      </c>
+      <c r="J43" t="s">
+        <v>390</v>
+      </c>
+      <c r="K43" t="s">
+        <v>391</v>
+      </c>
+      <c r="L43" t="s">
+        <v>75</v>
+      </c>
+      <c r="M43" t="s">
+        <v>392</v>
+      </c>
+      <c r="N43" t="s">
+        <v>393</v>
+      </c>
+      <c r="O43" t="s">
+        <v>394</v>
+      </c>
+      <c r="P43" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" t="s">
+        <v>384</v>
+      </c>
+      <c r="B44" t="s">
+        <v>385</v>
+      </c>
+      <c r="C44" t="s">
+        <v>386</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s">
+        <v>387</v>
+      </c>
+      <c r="F44" t="s">
+        <v>388</v>
+      </c>
+      <c r="G44" t="s">
+        <v>389</v>
+      </c>
+      <c r="H44" t="s">
+        <v>50</v>
+      </c>
+      <c r="I44" t="s">
+        <v>389</v>
+      </c>
+      <c r="J44" t="s">
+        <v>390</v>
+      </c>
+      <c r="K44" t="s">
+        <v>391</v>
+      </c>
+      <c r="L44" t="s">
+        <v>75</v>
+      </c>
+      <c r="M44" t="s">
+        <v>392</v>
+      </c>
+      <c r="N44" t="s">
+        <v>393</v>
+      </c>
+      <c r="O44" t="s">
+        <v>394</v>
+      </c>
+      <c r="P44" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" t="s">
+        <v>384</v>
+      </c>
+      <c r="B45" t="s">
+        <v>385</v>
+      </c>
+      <c r="C45" t="s">
+        <v>386</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s">
+        <v>387</v>
+      </c>
+      <c r="F45" t="s">
+        <v>388</v>
+      </c>
+      <c r="G45" t="s">
+        <v>389</v>
+      </c>
+      <c r="H45" t="s">
+        <v>50</v>
+      </c>
+      <c r="I45" t="s">
+        <v>389</v>
+      </c>
+      <c r="J45" t="s">
+        <v>390</v>
+      </c>
+      <c r="K45" t="s">
+        <v>391</v>
+      </c>
+      <c r="L45" t="s">
+        <v>75</v>
+      </c>
+      <c r="M45" t="s">
+        <v>392</v>
+      </c>
+      <c r="N45" t="s">
+        <v>393</v>
+      </c>
+      <c r="O45" t="s">
+        <v>394</v>
+      </c>
+      <c r="P45" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" t="s">
+        <v>384</v>
+      </c>
+      <c r="B46" t="s">
+        <v>385</v>
+      </c>
+      <c r="C46" t="s">
+        <v>386</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
+        <v>387</v>
+      </c>
+      <c r="F46" t="s">
+        <v>388</v>
+      </c>
+      <c r="G46" t="s">
+        <v>389</v>
+      </c>
+      <c r="H46" t="s">
+        <v>50</v>
+      </c>
+      <c r="I46" t="s">
+        <v>389</v>
+      </c>
+      <c r="J46" t="s">
+        <v>390</v>
+      </c>
+      <c r="K46" t="s">
+        <v>391</v>
+      </c>
+      <c r="L46" t="s">
+        <v>75</v>
+      </c>
+      <c r="M46" t="s">
+        <v>392</v>
+      </c>
+      <c r="N46" t="s">
+        <v>393</v>
+      </c>
+      <c r="O46" t="s">
+        <v>394</v>
+      </c>
+      <c r="P46" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" t="s">
+        <v>384</v>
+      </c>
+      <c r="B47" t="s">
+        <v>385</v>
+      </c>
+      <c r="C47" t="s">
+        <v>386</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" t="s">
+        <v>387</v>
+      </c>
+      <c r="F47" t="s">
+        <v>388</v>
+      </c>
+      <c r="G47" t="s">
+        <v>389</v>
+      </c>
+      <c r="H47" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" t="s">
+        <v>389</v>
+      </c>
+      <c r="J47" t="s">
+        <v>390</v>
+      </c>
+      <c r="K47" t="s">
+        <v>391</v>
+      </c>
+      <c r="L47" t="s">
+        <v>75</v>
+      </c>
+      <c r="M47" t="s">
+        <v>392</v>
+      </c>
+      <c r="N47" t="s">
+        <v>393</v>
+      </c>
+      <c r="O47" t="s">
+        <v>394</v>
+      </c>
+      <c r="P47" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" t="s">
+        <v>384</v>
+      </c>
+      <c r="B48" t="s">
+        <v>385</v>
+      </c>
+      <c r="C48" t="s">
+        <v>386</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" t="s">
+        <v>387</v>
+      </c>
+      <c r="F48" t="s">
+        <v>388</v>
+      </c>
+      <c r="G48" t="s">
+        <v>389</v>
+      </c>
+      <c r="H48" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48" t="s">
+        <v>389</v>
+      </c>
+      <c r="J48" t="s">
+        <v>390</v>
+      </c>
+      <c r="K48" t="s">
+        <v>391</v>
+      </c>
+      <c r="L48" t="s">
+        <v>75</v>
+      </c>
+      <c r="M48" t="s">
+        <v>392</v>
+      </c>
+      <c r="N48" t="s">
+        <v>393</v>
+      </c>
+      <c r="O48" t="s">
+        <v>394</v>
+      </c>
+      <c r="P48" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
+      <c r="A49" t="s">
+        <v>384</v>
+      </c>
+      <c r="B49" t="s">
+        <v>385</v>
+      </c>
+      <c r="C49" t="s">
+        <v>386</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" t="s">
+        <v>387</v>
+      </c>
+      <c r="F49" t="s">
+        <v>388</v>
+      </c>
+      <c r="G49" t="s">
+        <v>389</v>
+      </c>
+      <c r="H49" t="s">
+        <v>50</v>
+      </c>
+      <c r="I49" t="s">
+        <v>389</v>
+      </c>
+      <c r="J49" t="s">
+        <v>390</v>
+      </c>
+      <c r="K49" t="s">
+        <v>391</v>
+      </c>
+      <c r="L49" t="s">
+        <v>75</v>
+      </c>
+      <c r="M49" t="s">
+        <v>392</v>
+      </c>
+      <c r="N49" t="s">
+        <v>393</v>
+      </c>
+      <c r="O49" t="s">
+        <v>394</v>
+      </c>
+      <c r="P49" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50" t="s">
+        <v>384</v>
+      </c>
+      <c r="B50" t="s">
+        <v>385</v>
+      </c>
+      <c r="C50" t="s">
+        <v>386</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" t="s">
+        <v>387</v>
+      </c>
+      <c r="F50" t="s">
+        <v>388</v>
+      </c>
+      <c r="G50" t="s">
+        <v>389</v>
+      </c>
+      <c r="H50" t="s">
+        <v>50</v>
+      </c>
+      <c r="I50" t="s">
+        <v>389</v>
+      </c>
+      <c r="J50" t="s">
+        <v>390</v>
+      </c>
+      <c r="K50" t="s">
+        <v>391</v>
+      </c>
+      <c r="L50" t="s">
+        <v>75</v>
+      </c>
+      <c r="M50" t="s">
+        <v>392</v>
+      </c>
+      <c r="N50" t="s">
+        <v>393</v>
+      </c>
+      <c r="O50" t="s">
+        <v>394</v>
+      </c>
+      <c r="P50" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="A51" t="s">
+        <v>384</v>
+      </c>
+      <c r="B51" t="s">
+        <v>385</v>
+      </c>
+      <c r="C51" t="s">
+        <v>386</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" t="s">
+        <v>387</v>
+      </c>
+      <c r="F51" t="s">
+        <v>388</v>
+      </c>
+      <c r="G51" t="s">
+        <v>389</v>
+      </c>
+      <c r="H51" t="s">
+        <v>50</v>
+      </c>
+      <c r="I51" t="s">
+        <v>389</v>
+      </c>
+      <c r="J51" t="s">
+        <v>390</v>
+      </c>
+      <c r="K51" t="s">
+        <v>391</v>
+      </c>
+      <c r="L51" t="s">
+        <v>75</v>
+      </c>
+      <c r="M51" t="s">
+        <v>392</v>
+      </c>
+      <c r="N51" t="s">
+        <v>393</v>
+      </c>
+      <c r="O51" t="s">
+        <v>394</v>
+      </c>
+      <c r="P51" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="A52" t="s">
+        <v>384</v>
+      </c>
+      <c r="B52" t="s">
+        <v>385</v>
+      </c>
+      <c r="C52" t="s">
+        <v>386</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>387</v>
+      </c>
+      <c r="F52" t="s">
+        <v>388</v>
+      </c>
+      <c r="G52" t="s">
+        <v>389</v>
+      </c>
+      <c r="H52" t="s">
+        <v>50</v>
+      </c>
+      <c r="I52" t="s">
+        <v>389</v>
+      </c>
+      <c r="J52" t="s">
+        <v>390</v>
+      </c>
+      <c r="K52" t="s">
+        <v>391</v>
+      </c>
+      <c r="L52" t="s">
+        <v>75</v>
+      </c>
+      <c r="M52" t="s">
+        <v>392</v>
+      </c>
+      <c r="N52" t="s">
+        <v>393</v>
+      </c>
+      <c r="O52" t="s">
+        <v>394</v>
+      </c>
+      <c r="P52" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53" t="s">
+        <v>384</v>
+      </c>
+      <c r="B53" t="s">
+        <v>385</v>
+      </c>
+      <c r="C53" t="s">
+        <v>386</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" t="s">
+        <v>387</v>
+      </c>
+      <c r="F53" t="s">
+        <v>388</v>
+      </c>
+      <c r="G53" t="s">
+        <v>389</v>
+      </c>
+      <c r="H53" t="s">
+        <v>50</v>
+      </c>
+      <c r="I53" t="s">
+        <v>389</v>
+      </c>
+      <c r="J53" t="s">
+        <v>390</v>
+      </c>
+      <c r="K53" t="s">
+        <v>391</v>
+      </c>
+      <c r="L53" t="s">
+        <v>75</v>
+      </c>
+      <c r="M53" t="s">
+        <v>392</v>
+      </c>
+      <c r="N53" t="s">
+        <v>393</v>
+      </c>
+      <c r="O53" t="s">
+        <v>394</v>
+      </c>
+      <c r="P53" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54" t="s">
+        <v>384</v>
+      </c>
+      <c r="B54" t="s">
+        <v>385</v>
+      </c>
+      <c r="C54" t="s">
+        <v>386</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>387</v>
+      </c>
+      <c r="F54" t="s">
+        <v>388</v>
+      </c>
+      <c r="G54" t="s">
+        <v>389</v>
+      </c>
+      <c r="H54" t="s">
+        <v>50</v>
+      </c>
+      <c r="I54" t="s">
+        <v>389</v>
+      </c>
+      <c r="J54" t="s">
+        <v>390</v>
+      </c>
+      <c r="K54" t="s">
+        <v>391</v>
+      </c>
+      <c r="L54" t="s">
+        <v>75</v>
+      </c>
+      <c r="M54" t="s">
+        <v>392</v>
+      </c>
+      <c r="N54" t="s">
+        <v>393</v>
+      </c>
+      <c r="O54" t="s">
+        <v>394</v>
+      </c>
+      <c r="P54" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" t="s">
+        <v>384</v>
+      </c>
+      <c r="B55" t="s">
+        <v>385</v>
+      </c>
+      <c r="C55" t="s">
+        <v>386</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" t="s">
+        <v>387</v>
+      </c>
+      <c r="F55" t="s">
+        <v>388</v>
+      </c>
+      <c r="G55" t="s">
+        <v>389</v>
+      </c>
+      <c r="H55" t="s">
+        <v>50</v>
+      </c>
+      <c r="I55" t="s">
+        <v>389</v>
+      </c>
+      <c r="J55" t="s">
+        <v>390</v>
+      </c>
+      <c r="K55" t="s">
+        <v>391</v>
+      </c>
+      <c r="L55" t="s">
+        <v>75</v>
+      </c>
+      <c r="M55" t="s">
+        <v>392</v>
+      </c>
+      <c r="N55" t="s">
+        <v>393</v>
+      </c>
+      <c r="O55" t="s">
+        <v>394</v>
+      </c>
+      <c r="P55" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
+      <c r="A56" t="s">
+        <v>384</v>
+      </c>
+      <c r="B56" t="s">
+        <v>385</v>
+      </c>
+      <c r="C56" t="s">
+        <v>386</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>387</v>
+      </c>
+      <c r="F56" t="s">
+        <v>388</v>
+      </c>
+      <c r="G56" t="s">
+        <v>389</v>
+      </c>
+      <c r="H56" t="s">
+        <v>50</v>
+      </c>
+      <c r="I56" t="s">
+        <v>389</v>
+      </c>
+      <c r="J56" t="s">
+        <v>390</v>
+      </c>
+      <c r="K56" t="s">
+        <v>391</v>
+      </c>
+      <c r="L56" t="s">
+        <v>75</v>
+      </c>
+      <c r="M56" t="s">
+        <v>392</v>
+      </c>
+      <c r="N56" t="s">
+        <v>393</v>
+      </c>
+      <c r="O56" t="s">
+        <v>394</v>
+      </c>
+      <c r="P56" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="A57" t="s">
+        <v>384</v>
+      </c>
+      <c r="B57" t="s">
+        <v>385</v>
+      </c>
+      <c r="C57" t="s">
+        <v>386</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>387</v>
+      </c>
+      <c r="F57" t="s">
+        <v>388</v>
+      </c>
+      <c r="G57" t="s">
+        <v>389</v>
+      </c>
+      <c r="H57" t="s">
+        <v>50</v>
+      </c>
+      <c r="I57" t="s">
+        <v>389</v>
+      </c>
+      <c r="J57" t="s">
+        <v>390</v>
+      </c>
+      <c r="K57" t="s">
+        <v>391</v>
+      </c>
+      <c r="L57" t="s">
+        <v>75</v>
+      </c>
+      <c r="M57" t="s">
+        <v>392</v>
+      </c>
+      <c r="N57" t="s">
+        <v>393</v>
+      </c>
+      <c r="O57" t="s">
+        <v>394</v>
+      </c>
+      <c r="P57" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="A58" t="s">
+        <v>384</v>
+      </c>
+      <c r="B58" t="s">
+        <v>385</v>
+      </c>
+      <c r="C58" t="s">
+        <v>386</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s">
+        <v>387</v>
+      </c>
+      <c r="F58" t="s">
+        <v>388</v>
+      </c>
+      <c r="G58" t="s">
+        <v>389</v>
+      </c>
+      <c r="H58" t="s">
+        <v>50</v>
+      </c>
+      <c r="I58" t="s">
+        <v>389</v>
+      </c>
+      <c r="J58" t="s">
+        <v>390</v>
+      </c>
+      <c r="K58" t="s">
+        <v>391</v>
+      </c>
+      <c r="L58" t="s">
+        <v>75</v>
+      </c>
+      <c r="M58" t="s">
+        <v>392</v>
+      </c>
+      <c r="N58" t="s">
+        <v>393</v>
+      </c>
+      <c r="O58" t="s">
+        <v>394</v>
+      </c>
+      <c r="P58" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="A59" t="s">
+        <v>384</v>
+      </c>
+      <c r="B59" t="s">
+        <v>385</v>
+      </c>
+      <c r="C59" t="s">
+        <v>386</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" t="s">
+        <v>387</v>
+      </c>
+      <c r="F59" t="s">
+        <v>388</v>
+      </c>
+      <c r="G59" t="s">
+        <v>389</v>
+      </c>
+      <c r="H59" t="s">
+        <v>50</v>
+      </c>
+      <c r="I59" t="s">
+        <v>389</v>
+      </c>
+      <c r="J59" t="s">
+        <v>390</v>
+      </c>
+      <c r="K59" t="s">
+        <v>391</v>
+      </c>
+      <c r="L59" t="s">
+        <v>75</v>
+      </c>
+      <c r="M59" t="s">
+        <v>392</v>
+      </c>
+      <c r="N59" t="s">
+        <v>393</v>
+      </c>
+      <c r="O59" t="s">
+        <v>394</v>
+      </c>
+      <c r="P59" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="A60" t="s">
+        <v>384</v>
+      </c>
+      <c r="B60" t="s">
+        <v>385</v>
+      </c>
+      <c r="C60" t="s">
+        <v>386</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" t="s">
+        <v>387</v>
+      </c>
+      <c r="F60" t="s">
+        <v>388</v>
+      </c>
+      <c r="G60" t="s">
+        <v>389</v>
+      </c>
+      <c r="H60" t="s">
+        <v>50</v>
+      </c>
+      <c r="I60" t="s">
+        <v>389</v>
+      </c>
+      <c r="J60" t="s">
+        <v>390</v>
+      </c>
+      <c r="K60" t="s">
+        <v>391</v>
+      </c>
+      <c r="L60" t="s">
+        <v>75</v>
+      </c>
+      <c r="M60" t="s">
+        <v>392</v>
+      </c>
+      <c r="N60" t="s">
+        <v>393</v>
+      </c>
+      <c r="O60" t="s">
+        <v>394</v>
+      </c>
+      <c r="P60" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61" t="s">
+        <v>384</v>
+      </c>
+      <c r="B61" t="s">
+        <v>385</v>
+      </c>
+      <c r="C61" t="s">
+        <v>386</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" t="s">
+        <v>387</v>
+      </c>
+      <c r="F61" t="s">
+        <v>388</v>
+      </c>
+      <c r="G61" t="s">
+        <v>389</v>
+      </c>
+      <c r="H61" t="s">
+        <v>50</v>
+      </c>
+      <c r="I61" t="s">
+        <v>389</v>
+      </c>
+      <c r="J61" t="s">
+        <v>390</v>
+      </c>
+      <c r="K61" t="s">
+        <v>391</v>
+      </c>
+      <c r="L61" t="s">
+        <v>75</v>
+      </c>
+      <c r="M61" t="s">
+        <v>392</v>
+      </c>
+      <c r="N61" t="s">
+        <v>393</v>
+      </c>
+      <c r="O61" t="s">
+        <v>394</v>
+      </c>
+      <c r="P61" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="A62" t="s">
+        <v>384</v>
+      </c>
+      <c r="B62" t="s">
+        <v>385</v>
+      </c>
+      <c r="C62" t="s">
+        <v>386</v>
+      </c>
+      <c r="D62" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" t="s">
+        <v>387</v>
+      </c>
+      <c r="F62" t="s">
+        <v>388</v>
+      </c>
+      <c r="G62" t="s">
+        <v>389</v>
+      </c>
+      <c r="H62" t="s">
+        <v>50</v>
+      </c>
+      <c r="I62" t="s">
+        <v>389</v>
+      </c>
+      <c r="J62" t="s">
+        <v>390</v>
+      </c>
+      <c r="K62" t="s">
+        <v>391</v>
+      </c>
+      <c r="L62" t="s">
+        <v>75</v>
+      </c>
+      <c r="M62" t="s">
+        <v>392</v>
+      </c>
+      <c r="N62" t="s">
+        <v>393</v>
+      </c>
+      <c r="O62" t="s">
+        <v>394</v>
+      </c>
+      <c r="P62" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="A63" t="s">
+        <v>384</v>
+      </c>
+      <c r="B63" t="s">
+        <v>385</v>
+      </c>
+      <c r="C63" t="s">
+        <v>386</v>
+      </c>
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F63" t="s">
+        <v>388</v>
+      </c>
+      <c r="G63" t="s">
+        <v>389</v>
+      </c>
+      <c r="H63" t="s">
+        <v>50</v>
+      </c>
+      <c r="I63" t="s">
+        <v>389</v>
+      </c>
+      <c r="J63" t="s">
+        <v>390</v>
+      </c>
+      <c r="K63" t="s">
+        <v>391</v>
+      </c>
+      <c r="L63" t="s">
+        <v>75</v>
+      </c>
+      <c r="M63" t="s">
+        <v>392</v>
+      </c>
+      <c r="N63" t="s">
+        <v>393</v>
+      </c>
+      <c r="O63" t="s">
+        <v>394</v>
+      </c>
+      <c r="P63" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
+      <c r="A64" t="s">
+        <v>384</v>
+      </c>
+      <c r="B64" t="s">
+        <v>385</v>
+      </c>
+      <c r="C64" t="s">
+        <v>386</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" t="s">
+        <v>387</v>
+      </c>
+      <c r="F64" t="s">
+        <v>388</v>
+      </c>
+      <c r="G64" t="s">
+        <v>389</v>
+      </c>
+      <c r="H64" t="s">
+        <v>50</v>
+      </c>
+      <c r="I64" t="s">
+        <v>389</v>
+      </c>
+      <c r="J64" t="s">
+        <v>390</v>
+      </c>
+      <c r="K64" t="s">
+        <v>391</v>
+      </c>
+      <c r="L64" t="s">
+        <v>75</v>
+      </c>
+      <c r="M64" t="s">
+        <v>392</v>
+      </c>
+      <c r="N64" t="s">
+        <v>393</v>
+      </c>
+      <c r="O64" t="s">
+        <v>394</v>
+      </c>
+      <c r="P64" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
+      <c r="A65" t="s">
+        <v>384</v>
+      </c>
+      <c r="B65" t="s">
+        <v>385</v>
+      </c>
+      <c r="C65" t="s">
+        <v>386</v>
+      </c>
+      <c r="D65" t="s">
+        <v>14</v>
+      </c>
+      <c r="E65" t="s">
+        <v>387</v>
+      </c>
+      <c r="F65" t="s">
+        <v>388</v>
+      </c>
+      <c r="G65" t="s">
+        <v>389</v>
+      </c>
+      <c r="H65" t="s">
+        <v>50</v>
+      </c>
+      <c r="I65" t="s">
+        <v>389</v>
+      </c>
+      <c r="J65" t="s">
+        <v>390</v>
+      </c>
+      <c r="K65" t="s">
+        <v>391</v>
+      </c>
+      <c r="L65" t="s">
+        <v>75</v>
+      </c>
+      <c r="M65" t="s">
+        <v>392</v>
+      </c>
+      <c r="N65" t="s">
+        <v>393</v>
+      </c>
+      <c r="O65" t="s">
+        <v>394</v>
+      </c>
+      <c r="P65" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
+      <c r="A66" t="s">
+        <v>384</v>
+      </c>
+      <c r="B66" t="s">
+        <v>385</v>
+      </c>
+      <c r="C66" t="s">
+        <v>386</v>
+      </c>
+      <c r="D66" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" t="s">
+        <v>387</v>
+      </c>
+      <c r="F66" t="s">
+        <v>388</v>
+      </c>
+      <c r="G66" t="s">
+        <v>389</v>
+      </c>
+      <c r="H66" t="s">
+        <v>50</v>
+      </c>
+      <c r="I66" t="s">
+        <v>389</v>
+      </c>
+      <c r="J66" t="s">
+        <v>390</v>
+      </c>
+      <c r="K66" t="s">
+        <v>391</v>
+      </c>
+      <c r="L66" t="s">
+        <v>75</v>
+      </c>
+      <c r="M66" t="s">
+        <v>392</v>
+      </c>
+      <c r="N66" t="s">
+        <v>393</v>
+      </c>
+      <c r="O66" t="s">
+        <v>394</v>
+      </c>
+      <c r="P66" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
+      <c r="A67" t="s">
+        <v>384</v>
+      </c>
+      <c r="B67" t="s">
+        <v>385</v>
+      </c>
+      <c r="C67" t="s">
+        <v>386</v>
+      </c>
+      <c r="D67" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67" t="s">
+        <v>387</v>
+      </c>
+      <c r="F67" t="s">
+        <v>388</v>
+      </c>
+      <c r="G67" t="s">
+        <v>389</v>
+      </c>
+      <c r="H67" t="s">
+        <v>50</v>
+      </c>
+      <c r="I67" t="s">
+        <v>389</v>
+      </c>
+      <c r="J67" t="s">
+        <v>390</v>
+      </c>
+      <c r="K67" t="s">
+        <v>391</v>
+      </c>
+      <c r="L67" t="s">
+        <v>75</v>
+      </c>
+      <c r="M67" t="s">
+        <v>392</v>
+      </c>
+      <c r="N67" t="s">
+        <v>393</v>
+      </c>
+      <c r="O67" t="s">
+        <v>394</v>
+      </c>
+      <c r="P67" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="A68" t="s">
+        <v>384</v>
+      </c>
+      <c r="B68" t="s">
+        <v>385</v>
+      </c>
+      <c r="C68" t="s">
+        <v>386</v>
+      </c>
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" t="s">
+        <v>387</v>
+      </c>
+      <c r="F68" t="s">
+        <v>388</v>
+      </c>
+      <c r="G68" t="s">
+        <v>389</v>
+      </c>
+      <c r="H68" t="s">
+        <v>50</v>
+      </c>
+      <c r="I68" t="s">
+        <v>389</v>
+      </c>
+      <c r="J68" t="s">
+        <v>390</v>
+      </c>
+      <c r="K68" t="s">
+        <v>391</v>
+      </c>
+      <c r="L68" t="s">
+        <v>75</v>
+      </c>
+      <c r="M68" t="s">
+        <v>392</v>
+      </c>
+      <c r="N68" t="s">
+        <v>393</v>
+      </c>
+      <c r="O68" t="s">
+        <v>394</v>
+      </c>
+      <c r="P68" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
+      <c r="A69" t="s">
+        <v>384</v>
+      </c>
+      <c r="B69" t="s">
+        <v>385</v>
+      </c>
+      <c r="C69" t="s">
+        <v>386</v>
+      </c>
+      <c r="D69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" t="s">
+        <v>387</v>
+      </c>
+      <c r="F69" t="s">
+        <v>388</v>
+      </c>
+      <c r="G69" t="s">
+        <v>389</v>
+      </c>
+      <c r="H69" t="s">
+        <v>50</v>
+      </c>
+      <c r="I69" t="s">
+        <v>389</v>
+      </c>
+      <c r="J69" t="s">
+        <v>390</v>
+      </c>
+      <c r="K69" t="s">
+        <v>391</v>
+      </c>
+      <c r="L69" t="s">
+        <v>75</v>
+      </c>
+      <c r="M69" t="s">
+        <v>392</v>
+      </c>
+      <c r="N69" t="s">
+        <v>393</v>
+      </c>
+      <c r="O69" t="s">
+        <v>394</v>
+      </c>
+      <c r="P69" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
+      <c r="A70" t="s">
+        <v>384</v>
+      </c>
+      <c r="B70" t="s">
+        <v>385</v>
+      </c>
+      <c r="C70" t="s">
+        <v>386</v>
+      </c>
+      <c r="D70" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" t="s">
+        <v>387</v>
+      </c>
+      <c r="F70" t="s">
+        <v>388</v>
+      </c>
+      <c r="G70" t="s">
+        <v>389</v>
+      </c>
+      <c r="H70" t="s">
+        <v>50</v>
+      </c>
+      <c r="I70" t="s">
+        <v>389</v>
+      </c>
+      <c r="J70" t="s">
+        <v>390</v>
+      </c>
+      <c r="K70" t="s">
+        <v>391</v>
+      </c>
+      <c r="L70" t="s">
+        <v>75</v>
+      </c>
+      <c r="M70" t="s">
+        <v>392</v>
+      </c>
+      <c r="N70" t="s">
+        <v>393</v>
+      </c>
+      <c r="O70" t="s">
+        <v>394</v>
+      </c>
+      <c r="P70" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>394</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:I3"/>
@@ -4006,7 +5596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BE40"/>
+  <dimension ref="A1:OC61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="B20" xSplit="1" ySplit="4"/>
@@ -4022,17 +5612,17 @@
     <col customWidth="1" max="16384" min="35" style="27" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57">
+    <row r="1" spans="1:393">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="2" s="27" spans="1:57">
+    <row customHeight="1" ht="15.75" r="2" s="27" spans="1:393">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="16.5" r="3" s="27" spans="1:57">
+    <row customHeight="1" ht="16.5" r="3" s="27" spans="1:393">
       <c r="B3" s="20" t="s">
         <v>395</v>
       </c>
@@ -4098,7 +5688,7 @@
       <c r="BD3" s="21" t="n"/>
       <c r="BE3" s="22" t="n"/>
     </row>
-    <row r="4" spans="1:57">
+    <row r="4" spans="1:393">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -4271,7 +5861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:57">
+    <row r="5" spans="1:393">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4408,7 +5998,7 @@
         <v>5.145</v>
       </c>
     </row>
-    <row r="6" spans="1:57">
+    <row r="6" spans="1:393">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -4545,7 +6135,7 @@
         <v>5.145</v>
       </c>
     </row>
-    <row r="7" spans="1:57">
+    <row r="7" spans="1:393">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -4682,7 +6272,7 @@
         <v>5.307</v>
       </c>
     </row>
-    <row r="8" spans="1:57">
+    <row r="8" spans="1:393">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -4819,7 +6409,7 @@
         <v>5.275</v>
       </c>
     </row>
-    <row r="9" spans="1:57">
+    <row r="9" spans="1:393">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -4956,7 +6546,7 @@
         <v>5.08</v>
       </c>
     </row>
-    <row r="10" spans="1:57">
+    <row r="10" spans="1:393">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -5093,7 +6683,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="11" spans="1:57">
+    <row r="11" spans="1:393">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -5230,7 +6820,7 @@
         <v>5.242</v>
       </c>
     </row>
-    <row r="12" spans="1:57">
+    <row r="12" spans="1:393">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -5367,7 +6957,7 @@
         <v>5.278</v>
       </c>
     </row>
-    <row r="13" spans="1:57">
+    <row r="13" spans="1:393">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -5504,7 +7094,7 @@
         <v>5.295</v>
       </c>
     </row>
-    <row r="14" spans="1:57">
+    <row r="14" spans="1:393">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -5641,7 +7231,7 @@
         <v>5.268</v>
       </c>
     </row>
-    <row r="15" spans="1:57">
+    <row r="15" spans="1:393">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -5778,7 +7368,7 @@
         <v>5.191</v>
       </c>
     </row>
-    <row r="16" spans="1:57">
+    <row r="16" spans="1:393">
       <c r="A16" t="s">
         <v>145</v>
       </c>
@@ -5915,7 +7505,7 @@
         <v>5.044</v>
       </c>
     </row>
-    <row r="17" spans="1:57">
+    <row r="17" spans="1:393">
       <c r="A17" t="s">
         <v>159</v>
       </c>
@@ -6052,7 +7642,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="18" spans="1:57">
+    <row r="18" spans="1:393">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -6189,7 +7779,7 @@
         <v>5.075</v>
       </c>
     </row>
-    <row r="19" spans="1:57">
+    <row r="19" spans="1:393">
       <c r="A19" t="s">
         <v>186</v>
       </c>
@@ -6326,7 +7916,7 @@
         <v>5.205</v>
       </c>
     </row>
-    <row r="20" spans="1:57">
+    <row r="20" spans="1:393">
       <c r="A20" t="s">
         <v>199</v>
       </c>
@@ -6463,7 +8053,7 @@
         <v>5.229</v>
       </c>
     </row>
-    <row r="21" spans="1:57">
+    <row r="21" spans="1:393">
       <c r="A21" t="s">
         <v>213</v>
       </c>
@@ -6582,7 +8172,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="22" spans="1:57">
+    <row r="22" spans="1:393">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -6701,7 +8291,7 @@
         <v>5.315</v>
       </c>
     </row>
-    <row r="23" spans="1:57">
+    <row r="23" spans="1:393">
       <c r="A23" t="s">
         <v>238</v>
       </c>
@@ -6820,7 +8410,7 @@
         <v>5.08</v>
       </c>
     </row>
-    <row r="24" spans="1:57">
+    <row r="24" spans="1:393">
       <c r="A24" t="s">
         <v>251</v>
       </c>
@@ -6939,7 +8529,7 @@
         <v>4.81</v>
       </c>
     </row>
-    <row r="25" spans="1:57">
+    <row r="25" spans="1:393">
       <c r="A25" t="s">
         <v>263</v>
       </c>
@@ -7058,7 +8648,7 @@
         <v>5.311</v>
       </c>
     </row>
-    <row r="26" spans="1:57">
+    <row r="26" spans="1:393">
       <c r="A26" t="s">
         <v>275</v>
       </c>
@@ -7177,7 +8767,7 @@
         <v>5.312</v>
       </c>
     </row>
-    <row r="27" spans="1:57">
+    <row r="27" spans="1:393">
       <c r="A27" t="s">
         <v>286</v>
       </c>
@@ -7296,7 +8886,7 @@
         <v>5.286</v>
       </c>
     </row>
-    <row r="28" spans="1:57">
+    <row r="28" spans="1:393">
       <c r="A28" t="s">
         <v>297</v>
       </c>
@@ -7415,7 +9005,7 @@
         <v>5.211</v>
       </c>
     </row>
-    <row r="29" spans="1:57">
+    <row r="29" spans="1:393">
       <c r="A29" t="s">
         <v>308</v>
       </c>
@@ -7534,7 +9124,7 @@
         <v>5.289</v>
       </c>
     </row>
-    <row r="30" spans="1:57">
+    <row r="30" spans="1:393">
       <c r="A30" t="s">
         <v>320</v>
       </c>
@@ -7653,7 +9243,7 @@
         <v>4.971</v>
       </c>
     </row>
-    <row r="31" spans="1:57">
+    <row r="31" spans="1:393">
       <c r="A31" t="s">
         <v>332</v>
       </c>
@@ -7772,7 +9362,7 @@
         <v>4.767</v>
       </c>
     </row>
-    <row r="32" spans="1:57">
+    <row r="32" spans="1:393">
       <c r="A32" t="s">
         <v>343</v>
       </c>
@@ -7891,7 +9481,7 @@
         <v>5.274</v>
       </c>
     </row>
-    <row r="33" spans="1:57">
+    <row r="33" spans="1:393">
       <c r="A33" t="s">
         <v>354</v>
       </c>
@@ -8010,7 +9600,7 @@
         <v>5.33</v>
       </c>
     </row>
-    <row r="34" spans="1:57">
+    <row r="34" spans="1:393">
       <c r="A34" t="s">
         <v>364</v>
       </c>
@@ -8129,7 +9719,7 @@
         <v>5.271</v>
       </c>
     </row>
-    <row r="35" spans="1:57">
+    <row r="35" spans="1:393">
       <c r="A35" t="s">
         <v>375</v>
       </c>
@@ -8248,7 +9838,7 @@
         <v>5.35</v>
       </c>
     </row>
-    <row r="36" spans="1:57">
+    <row r="36" spans="1:393">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -8367,7 +9957,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="37" spans="1:57">
+    <row r="37" spans="1:393">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -8486,7 +10076,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="38" spans="1:57">
+    <row r="38" spans="1:393">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -8605,7 +10195,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="39" spans="1:57">
+    <row r="39" spans="1:393">
       <c r="A39" t="s">
         <v>384</v>
       </c>
@@ -8724,7 +10314,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="40" spans="1:57">
+    <row r="40" spans="1:393">
       <c r="A40" t="s">
         <v>384</v>
       </c>
@@ -8840,6 +10430,2691 @@
         <v>462</v>
       </c>
       <c r="BE40" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:393">
+      <c r="A41" t="s">
+        <v>384</v>
+      </c>
+      <c r="B41" t="s">
+        <v>434</v>
+      </c>
+      <c r="C41" t="s">
+        <v>435</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>436</v>
+      </c>
+      <c r="H41" t="s">
+        <v>437</v>
+      </c>
+      <c r="I41" t="s">
+        <v>438</v>
+      </c>
+      <c r="J41" t="s">
+        <v>439</v>
+      </c>
+      <c r="K41" t="s">
+        <v>75</v>
+      </c>
+      <c r="N41" t="s">
+        <v>440</v>
+      </c>
+      <c r="O41" t="s">
+        <v>441</v>
+      </c>
+      <c r="P41" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>443</v>
+      </c>
+      <c r="S41" t="s">
+        <v>130</v>
+      </c>
+      <c r="U41" t="s">
+        <v>444</v>
+      </c>
+      <c r="V41" t="s">
+        <v>445</v>
+      </c>
+      <c r="W41" t="s">
+        <v>446</v>
+      </c>
+      <c r="X41" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN41" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP41" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ41" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR41" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS41" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW41" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX41" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY41" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ41" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD41" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE41" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="42" spans="1:393">
+      <c r="A42" t="s">
+        <v>384</v>
+      </c>
+      <c r="B42" t="s">
+        <v>434</v>
+      </c>
+      <c r="C42" t="s">
+        <v>435</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" t="s">
+        <v>436</v>
+      </c>
+      <c r="H42" t="s">
+        <v>437</v>
+      </c>
+      <c r="I42" t="s">
+        <v>438</v>
+      </c>
+      <c r="J42" t="s">
+        <v>439</v>
+      </c>
+      <c r="K42" t="s">
+        <v>75</v>
+      </c>
+      <c r="N42" t="s">
+        <v>440</v>
+      </c>
+      <c r="O42" t="s">
+        <v>441</v>
+      </c>
+      <c r="P42" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>443</v>
+      </c>
+      <c r="S42" t="s">
+        <v>130</v>
+      </c>
+      <c r="U42" t="s">
+        <v>444</v>
+      </c>
+      <c r="V42" t="s">
+        <v>445</v>
+      </c>
+      <c r="W42" t="s">
+        <v>446</v>
+      </c>
+      <c r="X42" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK42" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN42" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP42" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ42" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR42" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS42" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW42" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX42" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY42" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ42" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD42" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE42" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="43" spans="1:393">
+      <c r="A43" t="s">
+        <v>384</v>
+      </c>
+      <c r="B43" t="s">
+        <v>434</v>
+      </c>
+      <c r="C43" t="s">
+        <v>435</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" t="s">
+        <v>436</v>
+      </c>
+      <c r="H43" t="s">
+        <v>437</v>
+      </c>
+      <c r="I43" t="s">
+        <v>438</v>
+      </c>
+      <c r="J43" t="s">
+        <v>439</v>
+      </c>
+      <c r="K43" t="s">
+        <v>75</v>
+      </c>
+      <c r="N43" t="s">
+        <v>440</v>
+      </c>
+      <c r="O43" t="s">
+        <v>441</v>
+      </c>
+      <c r="P43" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>443</v>
+      </c>
+      <c r="S43" t="s">
+        <v>130</v>
+      </c>
+      <c r="U43" t="s">
+        <v>444</v>
+      </c>
+      <c r="V43" t="s">
+        <v>445</v>
+      </c>
+      <c r="W43" t="s">
+        <v>446</v>
+      </c>
+      <c r="X43" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK43" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP43" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ43" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR43" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS43" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW43" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX43" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY43" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ43" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD43" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE43" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="44" spans="1:393">
+      <c r="A44" t="s">
+        <v>384</v>
+      </c>
+      <c r="B44" t="s">
+        <v>434</v>
+      </c>
+      <c r="C44" t="s">
+        <v>435</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" t="s">
+        <v>436</v>
+      </c>
+      <c r="H44" t="s">
+        <v>437</v>
+      </c>
+      <c r="I44" t="s">
+        <v>438</v>
+      </c>
+      <c r="J44" t="s">
+        <v>439</v>
+      </c>
+      <c r="K44" t="s">
+        <v>75</v>
+      </c>
+      <c r="N44" t="s">
+        <v>440</v>
+      </c>
+      <c r="O44" t="s">
+        <v>441</v>
+      </c>
+      <c r="P44" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>443</v>
+      </c>
+      <c r="S44" t="s">
+        <v>130</v>
+      </c>
+      <c r="U44" t="s">
+        <v>444</v>
+      </c>
+      <c r="V44" t="s">
+        <v>445</v>
+      </c>
+      <c r="W44" t="s">
+        <v>446</v>
+      </c>
+      <c r="X44" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI44" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK44" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL44" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN44" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP44" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ44" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR44" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS44" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW44" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX44" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY44" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ44" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD44" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE44" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="45" spans="1:393">
+      <c r="A45" t="s">
+        <v>384</v>
+      </c>
+      <c r="B45" t="s">
+        <v>434</v>
+      </c>
+      <c r="C45" t="s">
+        <v>435</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" t="s">
+        <v>436</v>
+      </c>
+      <c r="H45" t="s">
+        <v>437</v>
+      </c>
+      <c r="I45" t="s">
+        <v>438</v>
+      </c>
+      <c r="J45" t="s">
+        <v>439</v>
+      </c>
+      <c r="K45" t="s">
+        <v>75</v>
+      </c>
+      <c r="N45" t="s">
+        <v>440</v>
+      </c>
+      <c r="O45" t="s">
+        <v>441</v>
+      </c>
+      <c r="P45" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>443</v>
+      </c>
+      <c r="S45" t="s">
+        <v>130</v>
+      </c>
+      <c r="U45" t="s">
+        <v>444</v>
+      </c>
+      <c r="V45" t="s">
+        <v>445</v>
+      </c>
+      <c r="W45" t="s">
+        <v>446</v>
+      </c>
+      <c r="X45" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG45" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ45" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK45" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN45" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP45" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ45" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR45" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS45" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW45" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX45" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY45" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ45" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD45" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE45" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:393">
+      <c r="A46" t="s">
+        <v>384</v>
+      </c>
+      <c r="B46" t="s">
+        <v>434</v>
+      </c>
+      <c r="C46" t="s">
+        <v>435</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" t="s">
+        <v>436</v>
+      </c>
+      <c r="H46" t="s">
+        <v>437</v>
+      </c>
+      <c r="I46" t="s">
+        <v>438</v>
+      </c>
+      <c r="J46" t="s">
+        <v>439</v>
+      </c>
+      <c r="K46" t="s">
+        <v>75</v>
+      </c>
+      <c r="N46" t="s">
+        <v>440</v>
+      </c>
+      <c r="O46" t="s">
+        <v>441</v>
+      </c>
+      <c r="P46" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>443</v>
+      </c>
+      <c r="S46" t="s">
+        <v>130</v>
+      </c>
+      <c r="U46" t="s">
+        <v>444</v>
+      </c>
+      <c r="V46" t="s">
+        <v>445</v>
+      </c>
+      <c r="W46" t="s">
+        <v>446</v>
+      </c>
+      <c r="X46" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK46" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN46" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP46" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ46" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR46" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS46" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW46" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX46" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY46" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ46" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD46" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE46" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="47" spans="1:393">
+      <c r="A47" t="s">
+        <v>384</v>
+      </c>
+      <c r="B47" t="s">
+        <v>434</v>
+      </c>
+      <c r="C47" t="s">
+        <v>435</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" t="s">
+        <v>436</v>
+      </c>
+      <c r="H47" t="s">
+        <v>437</v>
+      </c>
+      <c r="I47" t="s">
+        <v>438</v>
+      </c>
+      <c r="J47" t="s">
+        <v>439</v>
+      </c>
+      <c r="K47" t="s">
+        <v>75</v>
+      </c>
+      <c r="N47" t="s">
+        <v>440</v>
+      </c>
+      <c r="O47" t="s">
+        <v>441</v>
+      </c>
+      <c r="P47" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>443</v>
+      </c>
+      <c r="S47" t="s">
+        <v>130</v>
+      </c>
+      <c r="U47" t="s">
+        <v>444</v>
+      </c>
+      <c r="V47" t="s">
+        <v>445</v>
+      </c>
+      <c r="W47" t="s">
+        <v>446</v>
+      </c>
+      <c r="X47" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK47" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL47" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN47" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP47" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ47" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR47" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS47" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW47" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX47" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY47" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ47" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD47" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE47" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="48" spans="1:393">
+      <c r="A48" t="s">
+        <v>384</v>
+      </c>
+      <c r="B48" t="s">
+        <v>434</v>
+      </c>
+      <c r="C48" t="s">
+        <v>435</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
+        <v>436</v>
+      </c>
+      <c r="H48" t="s">
+        <v>437</v>
+      </c>
+      <c r="I48" t="s">
+        <v>438</v>
+      </c>
+      <c r="J48" t="s">
+        <v>439</v>
+      </c>
+      <c r="K48" t="s">
+        <v>75</v>
+      </c>
+      <c r="N48" t="s">
+        <v>440</v>
+      </c>
+      <c r="O48" t="s">
+        <v>441</v>
+      </c>
+      <c r="P48" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>443</v>
+      </c>
+      <c r="S48" t="s">
+        <v>130</v>
+      </c>
+      <c r="U48" t="s">
+        <v>444</v>
+      </c>
+      <c r="V48" t="s">
+        <v>445</v>
+      </c>
+      <c r="W48" t="s">
+        <v>446</v>
+      </c>
+      <c r="X48" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG48" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ48" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK48" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL48" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN48" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP48" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ48" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR48" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS48" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW48" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX48" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY48" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ48" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD48" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE48" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="49" spans="1:393">
+      <c r="A49" t="s">
+        <v>384</v>
+      </c>
+      <c r="B49" t="s">
+        <v>434</v>
+      </c>
+      <c r="C49" t="s">
+        <v>435</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" t="s">
+        <v>436</v>
+      </c>
+      <c r="H49" t="s">
+        <v>437</v>
+      </c>
+      <c r="I49" t="s">
+        <v>438</v>
+      </c>
+      <c r="J49" t="s">
+        <v>439</v>
+      </c>
+      <c r="K49" t="s">
+        <v>75</v>
+      </c>
+      <c r="N49" t="s">
+        <v>440</v>
+      </c>
+      <c r="O49" t="s">
+        <v>441</v>
+      </c>
+      <c r="P49" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>443</v>
+      </c>
+      <c r="S49" t="s">
+        <v>130</v>
+      </c>
+      <c r="U49" t="s">
+        <v>444</v>
+      </c>
+      <c r="V49" t="s">
+        <v>445</v>
+      </c>
+      <c r="W49" t="s">
+        <v>446</v>
+      </c>
+      <c r="X49" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI49" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK49" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL49" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN49" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP49" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ49" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR49" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS49" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW49" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX49" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY49" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ49" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD49" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE49" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="50" spans="1:393">
+      <c r="A50" t="s">
+        <v>384</v>
+      </c>
+      <c r="B50" t="s">
+        <v>434</v>
+      </c>
+      <c r="C50" t="s">
+        <v>435</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" t="s">
+        <v>436</v>
+      </c>
+      <c r="H50" t="s">
+        <v>437</v>
+      </c>
+      <c r="I50" t="s">
+        <v>438</v>
+      </c>
+      <c r="J50" t="s">
+        <v>439</v>
+      </c>
+      <c r="K50" t="s">
+        <v>75</v>
+      </c>
+      <c r="N50" t="s">
+        <v>440</v>
+      </c>
+      <c r="O50" t="s">
+        <v>441</v>
+      </c>
+      <c r="P50" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>443</v>
+      </c>
+      <c r="S50" t="s">
+        <v>130</v>
+      </c>
+      <c r="U50" t="s">
+        <v>444</v>
+      </c>
+      <c r="V50" t="s">
+        <v>445</v>
+      </c>
+      <c r="W50" t="s">
+        <v>446</v>
+      </c>
+      <c r="X50" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG50" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI50" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ50" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK50" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL50" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN50" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP50" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ50" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR50" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS50" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW50" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX50" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY50" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ50" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD50" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE50" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="51" spans="1:393">
+      <c r="A51" t="s">
+        <v>384</v>
+      </c>
+      <c r="B51" t="s">
+        <v>434</v>
+      </c>
+      <c r="C51" t="s">
+        <v>435</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" t="s">
+        <v>436</v>
+      </c>
+      <c r="H51" t="s">
+        <v>437</v>
+      </c>
+      <c r="I51" t="s">
+        <v>438</v>
+      </c>
+      <c r="J51" t="s">
+        <v>439</v>
+      </c>
+      <c r="K51" t="s">
+        <v>75</v>
+      </c>
+      <c r="N51" t="s">
+        <v>440</v>
+      </c>
+      <c r="O51" t="s">
+        <v>441</v>
+      </c>
+      <c r="P51" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>443</v>
+      </c>
+      <c r="S51" t="s">
+        <v>130</v>
+      </c>
+      <c r="U51" t="s">
+        <v>444</v>
+      </c>
+      <c r="V51" t="s">
+        <v>445</v>
+      </c>
+      <c r="W51" t="s">
+        <v>446</v>
+      </c>
+      <c r="X51" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI51" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ51" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK51" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL51" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN51" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP51" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ51" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR51" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS51" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW51" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX51" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY51" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ51" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD51" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE51" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="52" spans="1:393">
+      <c r="A52" t="s">
+        <v>384</v>
+      </c>
+      <c r="B52" t="s">
+        <v>434</v>
+      </c>
+      <c r="C52" t="s">
+        <v>435</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
+        <v>436</v>
+      </c>
+      <c r="H52" t="s">
+        <v>437</v>
+      </c>
+      <c r="I52" t="s">
+        <v>438</v>
+      </c>
+      <c r="J52" t="s">
+        <v>439</v>
+      </c>
+      <c r="K52" t="s">
+        <v>75</v>
+      </c>
+      <c r="N52" t="s">
+        <v>440</v>
+      </c>
+      <c r="O52" t="s">
+        <v>441</v>
+      </c>
+      <c r="P52" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>443</v>
+      </c>
+      <c r="S52" t="s">
+        <v>130</v>
+      </c>
+      <c r="U52" t="s">
+        <v>444</v>
+      </c>
+      <c r="V52" t="s">
+        <v>445</v>
+      </c>
+      <c r="W52" t="s">
+        <v>446</v>
+      </c>
+      <c r="X52" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI52" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ52" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK52" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL52" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN52" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP52" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ52" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR52" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS52" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW52" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX52" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY52" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ52" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD52" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE52" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="53" spans="1:393">
+      <c r="A53" t="s">
+        <v>384</v>
+      </c>
+      <c r="B53" t="s">
+        <v>434</v>
+      </c>
+      <c r="C53" t="s">
+        <v>435</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" t="s">
+        <v>436</v>
+      </c>
+      <c r="H53" t="s">
+        <v>437</v>
+      </c>
+      <c r="I53" t="s">
+        <v>438</v>
+      </c>
+      <c r="J53" t="s">
+        <v>439</v>
+      </c>
+      <c r="K53" t="s">
+        <v>75</v>
+      </c>
+      <c r="N53" t="s">
+        <v>440</v>
+      </c>
+      <c r="O53" t="s">
+        <v>441</v>
+      </c>
+      <c r="P53" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>443</v>
+      </c>
+      <c r="S53" t="s">
+        <v>130</v>
+      </c>
+      <c r="U53" t="s">
+        <v>444</v>
+      </c>
+      <c r="V53" t="s">
+        <v>445</v>
+      </c>
+      <c r="W53" t="s">
+        <v>446</v>
+      </c>
+      <c r="X53" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG53" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI53" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ53" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK53" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN53" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP53" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ53" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR53" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS53" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW53" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX53" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY53" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ53" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD53" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE53" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="54" spans="1:393">
+      <c r="A54" t="s">
+        <v>384</v>
+      </c>
+      <c r="B54" t="s">
+        <v>434</v>
+      </c>
+      <c r="C54" t="s">
+        <v>435</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" t="s">
+        <v>436</v>
+      </c>
+      <c r="H54" t="s">
+        <v>437</v>
+      </c>
+      <c r="I54" t="s">
+        <v>438</v>
+      </c>
+      <c r="J54" t="s">
+        <v>439</v>
+      </c>
+      <c r="K54" t="s">
+        <v>75</v>
+      </c>
+      <c r="N54" t="s">
+        <v>440</v>
+      </c>
+      <c r="O54" t="s">
+        <v>441</v>
+      </c>
+      <c r="P54" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>443</v>
+      </c>
+      <c r="S54" t="s">
+        <v>130</v>
+      </c>
+      <c r="U54" t="s">
+        <v>444</v>
+      </c>
+      <c r="V54" t="s">
+        <v>445</v>
+      </c>
+      <c r="W54" t="s">
+        <v>446</v>
+      </c>
+      <c r="X54" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI54" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ54" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK54" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL54" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN54" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP54" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ54" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR54" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS54" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW54" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX54" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY54" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ54" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD54" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE54" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="55" spans="1:393">
+      <c r="A55" t="s">
+        <v>384</v>
+      </c>
+      <c r="B55" t="s">
+        <v>434</v>
+      </c>
+      <c r="C55" t="s">
+        <v>435</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" t="s">
+        <v>436</v>
+      </c>
+      <c r="H55" t="s">
+        <v>437</v>
+      </c>
+      <c r="I55" t="s">
+        <v>438</v>
+      </c>
+      <c r="J55" t="s">
+        <v>439</v>
+      </c>
+      <c r="K55" t="s">
+        <v>75</v>
+      </c>
+      <c r="N55" t="s">
+        <v>440</v>
+      </c>
+      <c r="O55" t="s">
+        <v>441</v>
+      </c>
+      <c r="P55" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>443</v>
+      </c>
+      <c r="S55" t="s">
+        <v>130</v>
+      </c>
+      <c r="U55" t="s">
+        <v>444</v>
+      </c>
+      <c r="V55" t="s">
+        <v>445</v>
+      </c>
+      <c r="W55" t="s">
+        <v>446</v>
+      </c>
+      <c r="X55" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ55" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK55" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN55" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP55" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ55" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR55" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS55" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW55" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX55" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY55" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ55" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD55" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE55" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="56" spans="1:393">
+      <c r="A56" t="s">
+        <v>384</v>
+      </c>
+      <c r="B56" t="s">
+        <v>434</v>
+      </c>
+      <c r="C56" t="s">
+        <v>435</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" t="s">
+        <v>436</v>
+      </c>
+      <c r="H56" t="s">
+        <v>437</v>
+      </c>
+      <c r="I56" t="s">
+        <v>438</v>
+      </c>
+      <c r="J56" t="s">
+        <v>439</v>
+      </c>
+      <c r="K56" t="s">
+        <v>75</v>
+      </c>
+      <c r="N56" t="s">
+        <v>440</v>
+      </c>
+      <c r="O56" t="s">
+        <v>441</v>
+      </c>
+      <c r="P56" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>443</v>
+      </c>
+      <c r="S56" t="s">
+        <v>130</v>
+      </c>
+      <c r="U56" t="s">
+        <v>444</v>
+      </c>
+      <c r="V56" t="s">
+        <v>445</v>
+      </c>
+      <c r="W56" t="s">
+        <v>446</v>
+      </c>
+      <c r="X56" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD56" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG56" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI56" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ56" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK56" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL56" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN56" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP56" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ56" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR56" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS56" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW56" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX56" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY56" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ56" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD56" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE56" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="57" spans="1:393">
+      <c r="A57" t="s">
+        <v>384</v>
+      </c>
+      <c r="B57" t="s">
+        <v>434</v>
+      </c>
+      <c r="C57" t="s">
+        <v>435</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" t="s">
+        <v>436</v>
+      </c>
+      <c r="H57" t="s">
+        <v>437</v>
+      </c>
+      <c r="I57" t="s">
+        <v>438</v>
+      </c>
+      <c r="J57" t="s">
+        <v>439</v>
+      </c>
+      <c r="K57" t="s">
+        <v>75</v>
+      </c>
+      <c r="N57" t="s">
+        <v>440</v>
+      </c>
+      <c r="O57" t="s">
+        <v>441</v>
+      </c>
+      <c r="P57" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>443</v>
+      </c>
+      <c r="S57" t="s">
+        <v>130</v>
+      </c>
+      <c r="U57" t="s">
+        <v>444</v>
+      </c>
+      <c r="V57" t="s">
+        <v>445</v>
+      </c>
+      <c r="W57" t="s">
+        <v>446</v>
+      </c>
+      <c r="X57" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG57" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ57" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK57" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN57" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP57" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ57" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR57" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS57" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW57" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX57" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY57" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ57" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD57" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE57" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="58" spans="1:393">
+      <c r="A58" t="s">
+        <v>384</v>
+      </c>
+      <c r="B58" t="s">
+        <v>434</v>
+      </c>
+      <c r="I58" t="s">
+        <v>438</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW58" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF58" t="s">
+        <v>442</v>
+      </c>
+      <c r="BM58" t="s">
+        <v>446</v>
+      </c>
+      <c r="BN58" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU58" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV58" t="n">
+        <v>0</v>
+      </c>
+      <c r="CC58" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD58" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK58" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL58" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN58" t="s">
+        <v>437</v>
+      </c>
+      <c r="CS58" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT58" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU58" t="s">
+        <v>441</v>
+      </c>
+      <c r="DA58" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ58" t="s">
+        <v>451</v>
+      </c>
+      <c r="DQ58" t="s">
+        <v>451</v>
+      </c>
+      <c r="DR58" t="n">
+        <v>0</v>
+      </c>
+      <c r="DY58" t="n">
+        <v>0</v>
+      </c>
+      <c r="DZ58" t="n">
+        <v>0</v>
+      </c>
+      <c r="EG58" t="n">
+        <v>0</v>
+      </c>
+      <c r="EH58" t="n">
+        <v>0</v>
+      </c>
+      <c r="EO58" t="n">
+        <v>0</v>
+      </c>
+      <c r="EP58" t="n">
+        <v>0</v>
+      </c>
+      <c r="EW58" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX58" t="n">
+        <v>0</v>
+      </c>
+      <c r="FE58" t="n">
+        <v>0</v>
+      </c>
+      <c r="FN58" t="s">
+        <v>456</v>
+      </c>
+      <c r="FU58" t="s">
+        <v>460</v>
+      </c>
+      <c r="FV58" t="n">
+        <v>0</v>
+      </c>
+      <c r="GC58" t="n">
+        <v>0</v>
+      </c>
+      <c r="GD58" t="n">
+        <v>0</v>
+      </c>
+      <c r="GH58" t="s">
+        <v>445</v>
+      </c>
+      <c r="GK58" t="n">
+        <v>0</v>
+      </c>
+      <c r="GL58" t="n">
+        <v>0</v>
+      </c>
+      <c r="GO58" t="s">
+        <v>450</v>
+      </c>
+      <c r="GS58" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT58" t="n">
+        <v>0</v>
+      </c>
+      <c r="HA58" t="n">
+        <v>0</v>
+      </c>
+      <c r="HB58" t="n">
+        <v>0</v>
+      </c>
+      <c r="HI58" t="n">
+        <v>0</v>
+      </c>
+      <c r="KB58" t="s">
+        <v>454</v>
+      </c>
+      <c r="KI58" t="s">
+        <v>455</v>
+      </c>
+      <c r="NV58" t="s">
+        <v>459</v>
+      </c>
+      <c r="OC58" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="59" spans="1:393">
+      <c r="A59" t="s">
+        <v>384</v>
+      </c>
+      <c r="B59" t="s">
+        <v>434</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="s">
+        <v>437</v>
+      </c>
+      <c r="I59" t="s">
+        <v>438</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="s">
+        <v>441</v>
+      </c>
+      <c r="P59" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0</v>
+      </c>
+      <c r="R59" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="n">
+        <v>0</v>
+      </c>
+      <c r="T59" t="n">
+        <v>0</v>
+      </c>
+      <c r="U59" t="n">
+        <v>0</v>
+      </c>
+      <c r="V59" t="s">
+        <v>445</v>
+      </c>
+      <c r="W59" t="s">
+        <v>446</v>
+      </c>
+      <c r="X59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ59" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK59" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ59" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR59" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX59" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY59" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ59" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA59" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB59" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC59" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD59" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE59" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="60" spans="1:393">
+      <c r="A60" t="s">
+        <v>384</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>0</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" t="n">
+        <v>0</v>
+      </c>
+      <c r="T60" t="n">
+        <v>0</v>
+      </c>
+      <c r="U60" t="n">
+        <v>0</v>
+      </c>
+      <c r="V60" t="n">
+        <v>0</v>
+      </c>
+      <c r="W60" t="n">
+        <v>0</v>
+      </c>
+      <c r="X60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE60" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG60" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI60" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ60" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK60" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL60" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN60" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP60" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ60" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR60" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS60" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW60" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX60" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY60" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ60" t="s">
+        <v>461</v>
+      </c>
+      <c r="BD60" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE60" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="61" spans="1:393">
+      <c r="A61" t="s">
+        <v>384</v>
+      </c>
+      <c r="B61" t="s">
+        <v>434</v>
+      </c>
+      <c r="C61" t="s">
+        <v>435</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="s">
+        <v>436</v>
+      </c>
+      <c r="H61" t="s">
+        <v>437</v>
+      </c>
+      <c r="I61" t="s">
+        <v>438</v>
+      </c>
+      <c r="J61" t="s">
+        <v>439</v>
+      </c>
+      <c r="K61" t="s">
+        <v>75</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" t="s">
+        <v>440</v>
+      </c>
+      <c r="O61" t="s">
+        <v>441</v>
+      </c>
+      <c r="P61" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>443</v>
+      </c>
+      <c r="R61" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" t="s">
+        <v>130</v>
+      </c>
+      <c r="T61" t="n">
+        <v>0</v>
+      </c>
+      <c r="U61" t="s">
+        <v>444</v>
+      </c>
+      <c r="V61" t="s">
+        <v>445</v>
+      </c>
+      <c r="W61" t="s">
+        <v>446</v>
+      </c>
+      <c r="X61" t="s">
+        <v>447</v>
+      </c>
+      <c r="Y61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>228</v>
+      </c>
+      <c r="AF61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG61" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI61" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ61" t="s">
+        <v>454</v>
+      </c>
+      <c r="AK61" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL61" t="s">
+        <v>228</v>
+      </c>
+      <c r="AM61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN61" t="s">
+        <v>452</v>
+      </c>
+      <c r="AO61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP61" t="s">
+        <v>453</v>
+      </c>
+      <c r="AQ61" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR61" t="s">
+        <v>456</v>
+      </c>
+      <c r="AS61" t="s">
+        <v>457</v>
+      </c>
+      <c r="AT61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW61" t="s">
+        <v>458</v>
+      </c>
+      <c r="AX61" t="s">
+        <v>459</v>
+      </c>
+      <c r="AY61" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ61" t="s">
+        <v>461</v>
+      </c>
+      <c r="BA61" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB61" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC61" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD61" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE61" t="s">
         <v>463</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mapeada a energia armazeanda máxima com erro ao imprimir as saídas em xlsx
</commit_message>
<xml_diff>
--- a/IPDO.xlsx
+++ b/IPDO.xlsx
@@ -3,13 +3,13 @@
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:workbookPr codeName="ThisWorkbook"/>
   <s:bookViews>
-    <s:workbookView activeTab="0"/>
+    <s:workbookView activeTab="3"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="BalancoResumido" sheetId="1" r:id="rId1"/>
     <s:sheet name="BalancoDetalhado" sheetId="2" r:id="rId2"/>
     <s:sheet name="Intercambios" sheetId="3" r:id="rId3"/>
-    <s:sheet name="DadosComunsSIN" sheetId="4" r:id="rId4"/>
+    <s:sheet name="EnergiaPotencialArmazenada" sheetId="4" r:id="rId4"/>
     <s:sheet name="DemandaMaxima" sheetId="5" r:id="rId5"/>
   </s:sheets>
   <s:definedNames/>
@@ -1097,7 +1097,7 @@
   </sheetPr>
   <dimension ref="A3:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1293,84 +1293,269 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="B7" s="25" t="n"/>
-      <c r="C7" s="25" t="n"/>
-      <c r="D7" s="25" t="n"/>
-      <c r="E7" s="25" t="n"/>
-      <c r="F7" s="25" t="n"/>
-      <c r="G7" s="25" t="n"/>
-      <c r="I7" s="25" t="n"/>
-      <c r="J7" s="25" t="n"/>
-      <c r="K7" s="25" t="n"/>
-      <c r="L7" s="25" t="n"/>
-      <c r="M7" s="25" t="n"/>
-      <c r="N7" s="25" t="n"/>
-      <c r="O7" s="25" t="n"/>
-      <c r="Q7" s="25" t="n"/>
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="25" t="n">
+        <v>27.136</v>
+      </c>
+      <c r="C7" s="25" t="n">
+        <v>9.579000000000001</v>
+      </c>
+      <c r="D7" s="25" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E7" s="25" t="n">
+        <v>9.112</v>
+      </c>
+      <c r="F7" s="25" t="n">
+        <v>2.559</v>
+      </c>
+      <c r="G7" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="B8" s="25" t="n"/>
-      <c r="C8" s="25" t="n"/>
-      <c r="D8" s="25" t="n"/>
-      <c r="E8" s="25" t="n"/>
-      <c r="F8" s="25" t="n"/>
-      <c r="G8" s="25" t="n"/>
-      <c r="I8" s="25" t="n"/>
-      <c r="J8" s="25" t="n"/>
-      <c r="K8" s="25" t="n"/>
-      <c r="L8" s="25" t="n"/>
-      <c r="M8" s="25" t="n"/>
-      <c r="N8" s="25" t="n"/>
-      <c r="O8" s="25" t="n"/>
-      <c r="Q8" s="25" t="n"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="25" t="n">
+        <v>27.136</v>
+      </c>
+      <c r="C8" s="25" t="n">
+        <v>9.579000000000001</v>
+      </c>
+      <c r="D8" s="25" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E8" s="25" t="n">
+        <v>9.112</v>
+      </c>
+      <c r="F8" s="25" t="n">
+        <v>2.559</v>
+      </c>
+      <c r="G8" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="B9" s="25" t="n"/>
-      <c r="C9" s="25" t="n"/>
-      <c r="D9" s="25" t="n"/>
-      <c r="E9" s="25" t="n"/>
-      <c r="F9" s="25" t="n"/>
-      <c r="G9" s="25" t="n"/>
-      <c r="I9" s="25" t="n"/>
-      <c r="J9" s="25" t="n"/>
-      <c r="K9" s="25" t="n"/>
-      <c r="L9" s="25" t="n"/>
-      <c r="M9" s="25" t="n"/>
-      <c r="N9" s="25" t="n"/>
-      <c r="O9" s="25" t="n"/>
-      <c r="Q9" s="25" t="n"/>
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="25" t="n">
+        <v>27.136</v>
+      </c>
+      <c r="C9" s="25" t="n">
+        <v>9.579000000000001</v>
+      </c>
+      <c r="D9" s="25" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E9" s="25" t="n">
+        <v>9.112</v>
+      </c>
+      <c r="F9" s="25" t="n">
+        <v>2.559</v>
+      </c>
+      <c r="G9" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="B10" s="25" t="n"/>
-      <c r="C10" s="25" t="n"/>
-      <c r="D10" s="25" t="n"/>
-      <c r="E10" s="25" t="n"/>
-      <c r="F10" s="25" t="n"/>
-      <c r="G10" s="25" t="n"/>
-      <c r="I10" s="25" t="n"/>
-      <c r="J10" s="25" t="n"/>
-      <c r="K10" s="25" t="n"/>
-      <c r="L10" s="25" t="n"/>
-      <c r="M10" s="25" t="n"/>
-      <c r="N10" s="25" t="n"/>
-      <c r="O10" s="25" t="n"/>
-      <c r="Q10" s="25" t="n"/>
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="25" t="n">
+        <v>27.136</v>
+      </c>
+      <c r="C10" s="25" t="n">
+        <v>9.579000000000001</v>
+      </c>
+      <c r="D10" s="25" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E10" s="25" t="n">
+        <v>9.112</v>
+      </c>
+      <c r="F10" s="25" t="n">
+        <v>2.559</v>
+      </c>
+      <c r="G10" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="B11" s="25" t="n"/>
-      <c r="C11" s="25" t="n"/>
-      <c r="D11" s="25" t="n"/>
-      <c r="E11" s="25" t="n"/>
-      <c r="F11" s="25" t="n"/>
-      <c r="G11" s="25" t="n"/>
-      <c r="I11" s="25" t="n"/>
-      <c r="J11" s="25" t="n"/>
-      <c r="K11" s="25" t="n"/>
-      <c r="L11" s="25" t="n"/>
-      <c r="M11" s="25" t="n"/>
-      <c r="N11" s="25" t="n"/>
-      <c r="O11" s="25" t="n"/>
-      <c r="Q11" s="25" t="n"/>
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="25" t="n">
+        <v>27.136</v>
+      </c>
+      <c r="C11" s="25" t="n">
+        <v>9.579000000000001</v>
+      </c>
+      <c r="D11" s="25" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E11" s="25" t="n">
+        <v>9.112</v>
+      </c>
+      <c r="F11" s="25" t="n">
+        <v>2.559</v>
+      </c>
+      <c r="G11" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="25" t="n">
+        <v>50.376</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:17">
       <c r="B12" s="25" t="n"/>
@@ -1785,8 +1970,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="14" width="16.42578125"/>
-    <col customWidth="1" max="44" min="2" style="14" width="11.42578125"/>
-    <col customWidth="1" max="16384" min="45" style="14" width="11.42578125"/>
+    <col customWidth="1" max="45" min="2" style="14" width="11.42578125"/>
+    <col customWidth="1" max="16384" min="46" style="14" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:393">
@@ -7571,6 +7756,871 @@
         <v>6059</v>
       </c>
       <c r="BE36" t="n">
+        <v>4823</v>
+      </c>
+    </row>
+    <row r="37" spans="1:393">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="n">
+        <v>14161</v>
+      </c>
+      <c r="C37" t="n">
+        <v>4628</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>20779</v>
+      </c>
+      <c r="H37" t="n">
+        <v>28447</v>
+      </c>
+      <c r="I37" t="n">
+        <v>13657</v>
+      </c>
+      <c r="J37" t="n">
+        <v>4651</v>
+      </c>
+      <c r="K37" t="n">
+        <v>2015</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>20323</v>
+      </c>
+      <c r="O37" t="n">
+        <v>27085</v>
+      </c>
+      <c r="P37" t="n">
+        <v>6467</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>444</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>580</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>7491</v>
+      </c>
+      <c r="V37" t="n">
+        <v>7792</v>
+      </c>
+      <c r="W37" t="n">
+        <v>5781</v>
+      </c>
+      <c r="X37" t="n">
+        <v>567</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>250</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>6598</v>
+      </c>
+      <c r="AC37" t="n">
+        <v>7486</v>
+      </c>
+      <c r="AD37" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AE37" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AF37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AH37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI37" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AJ37" t="n">
+        <v>9285</v>
+      </c>
+      <c r="AK37" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AL37" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AM37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN37" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AO37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP37" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AQ37" t="n">
+        <v>9184</v>
+      </c>
+      <c r="AR37" t="n">
+        <v>4057</v>
+      </c>
+      <c r="AS37" t="n">
+        <v>1965</v>
+      </c>
+      <c r="AT37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW37" t="n">
+        <v>6022</v>
+      </c>
+      <c r="AX37" t="n">
+        <v>4852</v>
+      </c>
+      <c r="AY37" t="n">
+        <v>4108</v>
+      </c>
+      <c r="AZ37" t="n">
+        <v>1951</v>
+      </c>
+      <c r="BA37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD37" t="n">
+        <v>6059</v>
+      </c>
+      <c r="BE37" t="n">
+        <v>4823</v>
+      </c>
+    </row>
+    <row r="38" spans="1:393">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="n">
+        <v>14161</v>
+      </c>
+      <c r="C38" t="n">
+        <v>4628</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>20779</v>
+      </c>
+      <c r="H38" t="n">
+        <v>28447</v>
+      </c>
+      <c r="I38" t="n">
+        <v>13657</v>
+      </c>
+      <c r="J38" t="n">
+        <v>4651</v>
+      </c>
+      <c r="K38" t="n">
+        <v>2015</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>20323</v>
+      </c>
+      <c r="O38" t="n">
+        <v>27085</v>
+      </c>
+      <c r="P38" t="n">
+        <v>6467</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>444</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>580</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>7491</v>
+      </c>
+      <c r="V38" t="n">
+        <v>7792</v>
+      </c>
+      <c r="W38" t="n">
+        <v>5781</v>
+      </c>
+      <c r="X38" t="n">
+        <v>567</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>250</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>6598</v>
+      </c>
+      <c r="AC38" t="n">
+        <v>7486</v>
+      </c>
+      <c r="AD38" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AE38" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AF38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AH38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI38" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AJ38" t="n">
+        <v>9285</v>
+      </c>
+      <c r="AK38" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AL38" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AM38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN38" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AO38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP38" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AQ38" t="n">
+        <v>9184</v>
+      </c>
+      <c r="AR38" t="n">
+        <v>4057</v>
+      </c>
+      <c r="AS38" t="n">
+        <v>1965</v>
+      </c>
+      <c r="AT38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW38" t="n">
+        <v>6022</v>
+      </c>
+      <c r="AX38" t="n">
+        <v>4852</v>
+      </c>
+      <c r="AY38" t="n">
+        <v>4108</v>
+      </c>
+      <c r="AZ38" t="n">
+        <v>1951</v>
+      </c>
+      <c r="BA38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD38" t="n">
+        <v>6059</v>
+      </c>
+      <c r="BE38" t="n">
+        <v>4823</v>
+      </c>
+    </row>
+    <row r="39" spans="1:393">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="n">
+        <v>14161</v>
+      </c>
+      <c r="C39" t="n">
+        <v>4628</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>20779</v>
+      </c>
+      <c r="H39" t="n">
+        <v>28447</v>
+      </c>
+      <c r="I39" t="n">
+        <v>13657</v>
+      </c>
+      <c r="J39" t="n">
+        <v>4651</v>
+      </c>
+      <c r="K39" t="n">
+        <v>2015</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>20323</v>
+      </c>
+      <c r="O39" t="n">
+        <v>27085</v>
+      </c>
+      <c r="P39" t="n">
+        <v>6467</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>444</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" t="n">
+        <v>580</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" t="n">
+        <v>7491</v>
+      </c>
+      <c r="V39" t="n">
+        <v>7792</v>
+      </c>
+      <c r="W39" t="n">
+        <v>5781</v>
+      </c>
+      <c r="X39" t="n">
+        <v>567</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>250</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>6598</v>
+      </c>
+      <c r="AC39" t="n">
+        <v>7486</v>
+      </c>
+      <c r="AD39" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AE39" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AH39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI39" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AJ39" t="n">
+        <v>9285</v>
+      </c>
+      <c r="AK39" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AL39" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AM39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN39" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AO39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP39" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AQ39" t="n">
+        <v>9184</v>
+      </c>
+      <c r="AR39" t="n">
+        <v>4057</v>
+      </c>
+      <c r="AS39" t="n">
+        <v>1965</v>
+      </c>
+      <c r="AT39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW39" t="n">
+        <v>6022</v>
+      </c>
+      <c r="AX39" t="n">
+        <v>4852</v>
+      </c>
+      <c r="AY39" t="n">
+        <v>4108</v>
+      </c>
+      <c r="AZ39" t="n">
+        <v>1951</v>
+      </c>
+      <c r="BA39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD39" t="n">
+        <v>6059</v>
+      </c>
+      <c r="BE39" t="n">
+        <v>4823</v>
+      </c>
+    </row>
+    <row r="40" spans="1:393">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="n">
+        <v>14161</v>
+      </c>
+      <c r="C40" t="n">
+        <v>4628</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>20779</v>
+      </c>
+      <c r="H40" t="n">
+        <v>28447</v>
+      </c>
+      <c r="I40" t="n">
+        <v>13657</v>
+      </c>
+      <c r="J40" t="n">
+        <v>4651</v>
+      </c>
+      <c r="K40" t="n">
+        <v>2015</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>20323</v>
+      </c>
+      <c r="O40" t="n">
+        <v>27085</v>
+      </c>
+      <c r="P40" t="n">
+        <v>6467</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>444</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="n">
+        <v>580</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="n">
+        <v>7491</v>
+      </c>
+      <c r="V40" t="n">
+        <v>7792</v>
+      </c>
+      <c r="W40" t="n">
+        <v>5781</v>
+      </c>
+      <c r="X40" t="n">
+        <v>567</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>250</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB40" t="n">
+        <v>6598</v>
+      </c>
+      <c r="AC40" t="n">
+        <v>7486</v>
+      </c>
+      <c r="AD40" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AE40" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AF40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG40" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AH40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI40" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AJ40" t="n">
+        <v>9285</v>
+      </c>
+      <c r="AK40" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AL40" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AM40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN40" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AO40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP40" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AQ40" t="n">
+        <v>9184</v>
+      </c>
+      <c r="AR40" t="n">
+        <v>4057</v>
+      </c>
+      <c r="AS40" t="n">
+        <v>1965</v>
+      </c>
+      <c r="AT40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW40" t="n">
+        <v>6022</v>
+      </c>
+      <c r="AX40" t="n">
+        <v>4852</v>
+      </c>
+      <c r="AY40" t="n">
+        <v>4108</v>
+      </c>
+      <c r="AZ40" t="n">
+        <v>1951</v>
+      </c>
+      <c r="BA40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD40" t="n">
+        <v>6059</v>
+      </c>
+      <c r="BE40" t="n">
+        <v>4823</v>
+      </c>
+    </row>
+    <row r="41" spans="1:393">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="n">
+        <v>14161</v>
+      </c>
+      <c r="C41" t="n">
+        <v>4628</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>20779</v>
+      </c>
+      <c r="H41" t="n">
+        <v>28447</v>
+      </c>
+      <c r="I41" t="n">
+        <v>13657</v>
+      </c>
+      <c r="J41" t="n">
+        <v>4651</v>
+      </c>
+      <c r="K41" t="n">
+        <v>2015</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>20323</v>
+      </c>
+      <c r="O41" t="n">
+        <v>27085</v>
+      </c>
+      <c r="P41" t="n">
+        <v>6467</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>444</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="n">
+        <v>580</v>
+      </c>
+      <c r="T41" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" t="n">
+        <v>7491</v>
+      </c>
+      <c r="V41" t="n">
+        <v>7792</v>
+      </c>
+      <c r="W41" t="n">
+        <v>5781</v>
+      </c>
+      <c r="X41" t="n">
+        <v>567</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>250</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB41" t="n">
+        <v>6598</v>
+      </c>
+      <c r="AC41" t="n">
+        <v>7486</v>
+      </c>
+      <c r="AD41" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AE41" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AF41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG41" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AH41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI41" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AJ41" t="n">
+        <v>9285</v>
+      </c>
+      <c r="AK41" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AL41" t="n">
+        <v>1936</v>
+      </c>
+      <c r="AM41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN41" t="n">
+        <v>1728</v>
+      </c>
+      <c r="AO41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP41" t="n">
+        <v>6174</v>
+      </c>
+      <c r="AQ41" t="n">
+        <v>9184</v>
+      </c>
+      <c r="AR41" t="n">
+        <v>4057</v>
+      </c>
+      <c r="AS41" t="n">
+        <v>1965</v>
+      </c>
+      <c r="AT41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW41" t="n">
+        <v>6022</v>
+      </c>
+      <c r="AX41" t="n">
+        <v>4852</v>
+      </c>
+      <c r="AY41" t="n">
+        <v>4108</v>
+      </c>
+      <c r="AZ41" t="n">
+        <v>1951</v>
+      </c>
+      <c r="BA41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD41" t="n">
+        <v>6059</v>
+      </c>
+      <c r="BE41" t="n">
         <v>4823</v>
       </c>
     </row>
@@ -7805,8 +8855,8 @@
     <col bestFit="1" customWidth="1" max="342" min="342" style="14" width="5.5703125"/>
     <col customWidth="1" max="348" min="343" style="14" width="11.42578125"/>
     <col bestFit="1" customWidth="1" max="349" min="349" style="14" width="5.5703125"/>
-    <col customWidth="1" max="357" min="350" style="14" width="11.42578125"/>
-    <col customWidth="1" max="16384" min="358" style="14" width="11.42578125"/>
+    <col customWidth="1" max="358" min="350" style="14" width="11.42578125"/>
+    <col customWidth="1" max="16384" min="359" style="14" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:349">
@@ -7959,74 +9009,209 @@
       </c>
     </row>
     <row r="7" spans="1:349">
-      <c r="B7" s="10" t="n"/>
-      <c r="C7" s="10" t="n"/>
-      <c r="D7" s="10" t="n"/>
-      <c r="E7" s="10" t="n"/>
-      <c r="F7" s="10" t="n"/>
-      <c r="G7" s="10" t="n"/>
-      <c r="H7" s="11" t="n"/>
-      <c r="I7" s="11" t="n"/>
-      <c r="J7" s="11" t="n"/>
-      <c r="K7" s="11" t="n"/>
-      <c r="L7" s="11" t="n"/>
-      <c r="M7" s="11" t="n"/>
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>1236</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>3010</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>9424</v>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>1774</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>-888</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>1170</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>2780</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>9579</v>
+      </c>
+      <c r="K7" s="11" t="n">
+        <v>1610</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>-301</v>
+      </c>
+      <c r="M7" s="11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:349">
-      <c r="B8" s="10" t="n"/>
-      <c r="C8" s="10" t="n"/>
-      <c r="D8" s="10" t="n"/>
-      <c r="E8" s="10" t="n"/>
-      <c r="F8" s="10" t="n"/>
-      <c r="G8" s="10" t="n"/>
-      <c r="H8" s="11" t="n"/>
-      <c r="I8" s="11" t="n"/>
-      <c r="J8" s="11" t="n"/>
-      <c r="K8" s="11" t="n"/>
-      <c r="L8" s="11" t="n"/>
-      <c r="M8" s="11" t="n"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>1236</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>3010</v>
+      </c>
+      <c r="D8" s="10" t="n">
+        <v>9424</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>1774</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>-888</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11" t="n">
+        <v>1170</v>
+      </c>
+      <c r="I8" s="11" t="n">
+        <v>2780</v>
+      </c>
+      <c r="J8" s="11" t="n">
+        <v>9579</v>
+      </c>
+      <c r="K8" s="11" t="n">
+        <v>1610</v>
+      </c>
+      <c r="L8" s="11" t="n">
+        <v>-301</v>
+      </c>
+      <c r="M8" s="11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:349">
-      <c r="B9" s="10" t="n"/>
-      <c r="C9" s="10" t="n"/>
-      <c r="D9" s="10" t="n"/>
-      <c r="E9" s="10" t="n"/>
-      <c r="F9" s="10" t="n"/>
-      <c r="G9" s="10" t="n"/>
-      <c r="H9" s="11" t="n"/>
-      <c r="I9" s="11" t="n"/>
-      <c r="J9" s="11" t="n"/>
-      <c r="K9" s="11" t="n"/>
-      <c r="L9" s="11" t="n"/>
-      <c r="M9" s="11" t="n"/>
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>1236</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>3010</v>
+      </c>
+      <c r="D9" s="10" t="n">
+        <v>9424</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>1774</v>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>-888</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="n">
+        <v>1170</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>2780</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <v>9579</v>
+      </c>
+      <c r="K9" s="11" t="n">
+        <v>1610</v>
+      </c>
+      <c r="L9" s="11" t="n">
+        <v>-301</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:349">
-      <c r="B10" s="10" t="n"/>
-      <c r="C10" s="10" t="n"/>
-      <c r="D10" s="10" t="n"/>
-      <c r="E10" s="10" t="n"/>
-      <c r="F10" s="10" t="n"/>
-      <c r="G10" s="10" t="n"/>
-      <c r="H10" s="11" t="n"/>
-      <c r="I10" s="11" t="n"/>
-      <c r="J10" s="11" t="n"/>
-      <c r="K10" s="11" t="n"/>
-      <c r="L10" s="11" t="n"/>
-      <c r="M10" s="11" t="n"/>
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>1236</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>3010</v>
+      </c>
+      <c r="D10" s="10" t="n">
+        <v>9424</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>1774</v>
+      </c>
+      <c r="F10" s="10" t="n">
+        <v>-888</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <v>1170</v>
+      </c>
+      <c r="I10" s="11" t="n">
+        <v>2780</v>
+      </c>
+      <c r="J10" s="11" t="n">
+        <v>9579</v>
+      </c>
+      <c r="K10" s="11" t="n">
+        <v>1610</v>
+      </c>
+      <c r="L10" s="11" t="n">
+        <v>-301</v>
+      </c>
+      <c r="M10" s="11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:349">
-      <c r="B11" s="10" t="n"/>
-      <c r="C11" s="10" t="n"/>
-      <c r="D11" s="10" t="n"/>
-      <c r="E11" s="10" t="n"/>
-      <c r="F11" s="10" t="n"/>
-      <c r="G11" s="10" t="n"/>
-      <c r="H11" s="11" t="n"/>
-      <c r="I11" s="11" t="n"/>
-      <c r="J11" s="11" t="n"/>
-      <c r="K11" s="11" t="n"/>
-      <c r="L11" s="11" t="n"/>
-      <c r="M11" s="11" t="n"/>
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>1236</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>3010</v>
+      </c>
+      <c r="D11" s="10" t="n">
+        <v>9424</v>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>1774</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <v>-888</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11" t="n">
+        <v>1170</v>
+      </c>
+      <c r="I11" s="11" t="n">
+        <v>2780</v>
+      </c>
+      <c r="J11" s="11" t="n">
+        <v>9579</v>
+      </c>
+      <c r="K11" s="11" t="n">
+        <v>1610</v>
+      </c>
+      <c r="L11" s="11" t="n">
+        <v>-301</v>
+      </c>
+      <c r="M11" s="11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:349">
       <c r="B12" s="10" t="n"/>
@@ -8154,43 +9339,6 @@
       <c r="L20" s="13" t="n"/>
       <c r="M20" s="13" t="n"/>
     </row>
-    <row r="21" spans="1:349"/>
-    <row r="22" spans="1:349"/>
-    <row r="23" spans="1:349"/>
-    <row r="24" spans="1:349"/>
-    <row r="25" spans="1:349"/>
-    <row r="26" spans="1:349"/>
-    <row r="27" spans="1:349"/>
-    <row r="28" spans="1:349"/>
-    <row r="29" spans="1:349"/>
-    <row r="30" spans="1:349"/>
-    <row r="31" spans="1:349"/>
-    <row r="32" spans="1:349"/>
-    <row r="33" spans="1:349"/>
-    <row r="34" spans="1:349"/>
-    <row r="35" spans="1:349"/>
-    <row r="36" spans="1:349"/>
-    <row r="37" spans="1:349"/>
-    <row r="38" spans="1:349"/>
-    <row r="39" spans="1:349"/>
-    <row r="40" spans="1:349"/>
-    <row r="41" spans="1:349"/>
-    <row r="42" spans="1:349"/>
-    <row r="43" spans="1:349"/>
-    <row r="44" spans="1:349"/>
-    <row r="45" spans="1:349"/>
-    <row r="46" spans="1:349"/>
-    <row r="47" spans="1:349"/>
-    <row r="48" spans="1:349"/>
-    <row r="49" spans="1:349"/>
-    <row r="50" spans="1:349"/>
-    <row r="51" spans="1:349"/>
-    <row r="52" spans="1:349"/>
-    <row r="53" spans="1:349"/>
-    <row r="54" spans="1:349"/>
-    <row r="55" spans="1:349"/>
-    <row r="56" spans="1:349"/>
-    <row r="57" spans="1:349"/>
     <row r="58" spans="1:349">
       <c r="U58" t="s">
         <v>28</v>
@@ -8337,10 +9485,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8422,7 +9570,9 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="15" t="n"/>
+      <c r="A5" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="B5" s="25" t="n"/>
       <c r="C5" s="25" t="n"/>
       <c r="D5" s="25" t="n"/>
@@ -8435,6 +9585,11 @@
       <c r="K5" s="25" t="n"/>
       <c r="L5" s="25" t="n"/>
       <c r="M5" s="25" t="n"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>